<commit_message>
fix vsc control parameters
</commit_message>
<xml_diff>
--- a/stability_analysis/data/cases/IEEE_118_FULL_data_vsc.xlsx
+++ b/stability_analysis/data/cases/IEEE_118_FULL_data_vsc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francesca\Documents\StabilityAnalysis\stability_analysis\data\cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francesca\miniconda3\envs\gridcal_original\stability_analysis\stability_analysis\data\cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D4CBFF-00E8-4DB0-82AD-C2E3FFC42E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8042AA-1910-4DC2-B298-AD4A94A73E87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="922" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" tabRatio="922" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STATCOM" sheetId="4" r:id="rId1"/>
@@ -20,17 +20,6 @@
     <sheet name="MMC-Vdc-GFll" sheetId="22" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -657,14 +646,14 @@
       <selection activeCell="G16" sqref="G15:G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="6.6640625" style="4" customWidth="1"/>
-    <col min="3" max="52" width="6.6640625" style="1" customWidth="1"/>
-    <col min="53" max="16384" width="8.6640625" style="1"/>
+    <col min="1" max="2" width="6.7109375" style="4" customWidth="1"/>
+    <col min="3" max="52" width="6.7109375" style="1" customWidth="1"/>
+    <col min="53" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -757,7 +746,7 @@
       <c r="AX1" s="6"/>
       <c r="AY1" s="6"/>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:51" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -809,7 +798,7 @@
       <c r="AX2" s="2"/>
       <c r="AY2" s="2"/>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="2"/>
@@ -862,7 +851,7 @@
       <c r="AX3" s="2"/>
       <c r="AY3" s="2"/>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -915,7 +904,7 @@
       <c r="AX4" s="2"/>
       <c r="AY4" s="2"/>
     </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="8"/>
@@ -986,25 +975,25 @@
   <dimension ref="A1:AF352"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD28"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="6.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.6640625" style="1" customWidth="1"/>
-    <col min="9" max="10" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="5" width="6.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" style="1" customWidth="1"/>
+    <col min="9" max="10" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="50" width="6.6640625" style="1" customWidth="1"/>
-    <col min="51" max="16384" width="8.6640625" style="1"/>
+    <col min="14" max="14" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="50" width="6.7109375" style="1" customWidth="1"/>
+    <col min="51" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>55</v>
       </c>
@@ -1059,7 +1048,7 @@
       <c r="AE1" s="8"/>
       <c r="AF1" s="2"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>2E-3</v>
       </c>
@@ -1073,35 +1062,35 @@
         <v>0.15</v>
       </c>
       <c r="E2" s="7">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="F2" s="12">
         <v>1E-3</v>
       </c>
       <c r="G2" s="7">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="H2" s="7">
         <v>0.70699999999999996</v>
       </c>
       <c r="I2" s="16">
-        <v>1.1000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="J2" s="16">
-        <v>1.1000000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="K2" s="7">
         <f>1/10</f>
         <v>0.1</v>
       </c>
       <c r="L2" s="7">
-        <v>0.5</v>
+        <v>0.02</v>
       </c>
       <c r="M2" s="16">
         <v>0.1</v>
       </c>
       <c r="N2" s="7">
-        <v>2</v>
+        <v>0.02</v>
       </c>
       <c r="AB2" s="2"/>
       <c r="AC2" s="2"/>
@@ -1109,7 +1098,7 @@
       <c r="AE2" s="2"/>
       <c r="AF2" s="2"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -1125,7 +1114,7 @@
       <c r="M3" s="16"/>
       <c r="N3" s="7"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -1141,7 +1130,7 @@
       <c r="M4" s="16"/>
       <c r="N4" s="7"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -1157,7 +1146,7 @@
       <c r="M5" s="16"/>
       <c r="N5" s="7"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -1173,7 +1162,7 @@
       <c r="M6" s="16"/>
       <c r="N6" s="7"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1189,7 +1178,7 @@
       <c r="M7" s="16"/>
       <c r="N7" s="7"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -1205,7 +1194,7 @@
       <c r="M8" s="16"/>
       <c r="N8" s="7"/>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1221,7 +1210,7 @@
       <c r="M9" s="16"/>
       <c r="N9" s="7"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1237,7 +1226,7 @@
       <c r="M10" s="16"/>
       <c r="N10" s="7"/>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -1253,7 +1242,7 @@
       <c r="M11" s="16"/>
       <c r="N11" s="7"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -1269,7 +1258,7 @@
       <c r="M12" s="16"/>
       <c r="N12" s="7"/>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -1285,7 +1274,7 @@
       <c r="M13" s="16"/>
       <c r="N13" s="7"/>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -1301,7 +1290,7 @@
       <c r="M14" s="16"/>
       <c r="N14" s="7"/>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -1317,7 +1306,7 @@
       <c r="M15" s="16"/>
       <c r="N15" s="7"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -1333,7 +1322,7 @@
       <c r="M16" s="16"/>
       <c r="N16" s="7"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -1349,7 +1338,7 @@
       <c r="M17" s="16"/>
       <c r="N17" s="7"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -1365,7 +1354,7 @@
       <c r="M18" s="16"/>
       <c r="N18" s="7"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -1381,7 +1370,7 @@
       <c r="M19" s="16"/>
       <c r="N19" s="7"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -1397,7 +1386,7 @@
       <c r="M20" s="16"/>
       <c r="N20" s="7"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -1413,7 +1402,7 @@
       <c r="M21" s="16"/>
       <c r="N21" s="7"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -1429,7 +1418,7 @@
       <c r="M22" s="16"/>
       <c r="N22" s="7"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -1445,7 +1434,7 @@
       <c r="M23" s="16"/>
       <c r="N23" s="7"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -1461,7 +1450,7 @@
       <c r="M24" s="16"/>
       <c r="N24" s="7"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -1477,7 +1466,7 @@
       <c r="M25" s="16"/>
       <c r="N25" s="7"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -1493,7 +1482,7 @@
       <c r="M26" s="16"/>
       <c r="N26" s="7"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -1509,7 +1498,7 @@
       <c r="M27" s="16"/>
       <c r="N27" s="7"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -1525,1299 +1514,1299 @@
       <c r="M28" s="16"/>
       <c r="N28" s="7"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="I29" s="14"/>
       <c r="J29" s="14"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="I30" s="14"/>
       <c r="J30" s="14"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="I31" s="14"/>
       <c r="J31" s="14"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="I32" s="14"/>
       <c r="J32" s="14"/>
     </row>
-    <row r="33" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I33" s="14"/>
       <c r="J33" s="14"/>
     </row>
-    <row r="34" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I34" s="14"/>
       <c r="J34" s="14"/>
     </row>
-    <row r="35" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I35" s="14"/>
       <c r="J35" s="14"/>
     </row>
-    <row r="36" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I36" s="14"/>
       <c r="J36" s="14"/>
     </row>
-    <row r="37" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I37" s="14"/>
       <c r="J37" s="14"/>
     </row>
-    <row r="38" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I38" s="14"/>
       <c r="J38" s="14"/>
     </row>
-    <row r="39" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I39" s="14"/>
       <c r="J39" s="14"/>
     </row>
-    <row r="40" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I40" s="14"/>
       <c r="J40" s="14"/>
     </row>
-    <row r="41" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I41" s="14"/>
       <c r="J41" s="14"/>
     </row>
-    <row r="42" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I42" s="14"/>
       <c r="J42" s="14"/>
     </row>
-    <row r="43" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I43" s="14"/>
       <c r="J43" s="14"/>
     </row>
-    <row r="44" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I44" s="14"/>
       <c r="J44" s="14"/>
     </row>
-    <row r="45" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I45" s="14"/>
       <c r="J45" s="14"/>
     </row>
-    <row r="46" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I46" s="14"/>
       <c r="J46" s="14"/>
     </row>
-    <row r="47" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I47" s="14"/>
       <c r="J47" s="14"/>
     </row>
-    <row r="48" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I48" s="14"/>
       <c r="J48" s="14"/>
     </row>
-    <row r="49" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I49" s="14"/>
       <c r="J49" s="14"/>
     </row>
-    <row r="50" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I50" s="14"/>
       <c r="J50" s="14"/>
     </row>
-    <row r="51" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I51" s="14"/>
       <c r="J51" s="14"/>
     </row>
-    <row r="52" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I52" s="14"/>
       <c r="J52" s="14"/>
     </row>
-    <row r="53" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I53" s="14"/>
       <c r="J53" s="14"/>
     </row>
-    <row r="54" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I54" s="14"/>
       <c r="J54" s="14"/>
     </row>
-    <row r="55" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I55" s="14"/>
       <c r="J55" s="14"/>
     </row>
-    <row r="56" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I56" s="14"/>
       <c r="J56" s="14"/>
     </row>
-    <row r="57" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I57" s="14"/>
       <c r="J57" s="14"/>
     </row>
-    <row r="58" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I58" s="14"/>
       <c r="J58" s="14"/>
     </row>
-    <row r="59" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I59" s="14"/>
       <c r="J59" s="14"/>
     </row>
-    <row r="60" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I60" s="14"/>
       <c r="J60" s="14"/>
     </row>
-    <row r="61" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I61" s="14"/>
       <c r="J61" s="14"/>
     </row>
-    <row r="62" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I62" s="14"/>
       <c r="J62" s="14"/>
     </row>
-    <row r="63" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I63" s="14"/>
       <c r="J63" s="14"/>
     </row>
-    <row r="64" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I64" s="14"/>
       <c r="J64" s="14"/>
     </row>
-    <row r="65" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I65" s="14"/>
       <c r="J65" s="14"/>
     </row>
-    <row r="66" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I66" s="14"/>
       <c r="J66" s="14"/>
     </row>
-    <row r="67" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I67" s="14"/>
       <c r="J67" s="14"/>
     </row>
-    <row r="68" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I68" s="14"/>
       <c r="J68" s="14"/>
     </row>
-    <row r="69" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I69" s="14"/>
       <c r="J69" s="14"/>
     </row>
-    <row r="70" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I70" s="14"/>
       <c r="J70" s="14"/>
     </row>
-    <row r="71" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I71" s="14"/>
       <c r="J71" s="14"/>
     </row>
-    <row r="72" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I72" s="14"/>
       <c r="J72" s="14"/>
     </row>
-    <row r="73" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I73" s="14"/>
       <c r="J73" s="14"/>
     </row>
-    <row r="74" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I74" s="14"/>
       <c r="J74" s="14"/>
     </row>
-    <row r="75" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I75" s="14"/>
       <c r="J75" s="14"/>
     </row>
-    <row r="76" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I76" s="14"/>
       <c r="J76" s="14"/>
     </row>
-    <row r="77" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I77" s="14"/>
       <c r="J77" s="14"/>
     </row>
-    <row r="78" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I78" s="14"/>
       <c r="J78" s="14"/>
     </row>
-    <row r="79" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I79" s="14"/>
       <c r="J79" s="14"/>
     </row>
-    <row r="80" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I80" s="14"/>
       <c r="J80" s="14"/>
     </row>
-    <row r="81" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I81" s="14"/>
       <c r="J81" s="14"/>
     </row>
-    <row r="82" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I82" s="14"/>
       <c r="J82" s="14"/>
     </row>
-    <row r="83" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I83" s="14"/>
       <c r="J83" s="14"/>
     </row>
-    <row r="84" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I84" s="14"/>
       <c r="J84" s="14"/>
     </row>
-    <row r="85" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I85" s="14"/>
       <c r="J85" s="14"/>
     </row>
-    <row r="86" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I86" s="14"/>
       <c r="J86" s="14"/>
     </row>
-    <row r="87" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I87" s="14"/>
       <c r="J87" s="14"/>
     </row>
-    <row r="88" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I88" s="14"/>
       <c r="J88" s="14"/>
     </row>
-    <row r="89" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I89" s="14"/>
       <c r="J89" s="14"/>
     </row>
-    <row r="90" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I90" s="14"/>
       <c r="J90" s="14"/>
     </row>
-    <row r="91" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I91" s="14"/>
       <c r="J91" s="14"/>
     </row>
-    <row r="92" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I92" s="14"/>
       <c r="J92" s="14"/>
     </row>
-    <row r="93" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I93" s="14"/>
       <c r="J93" s="14"/>
     </row>
-    <row r="94" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I94" s="14"/>
       <c r="J94" s="14"/>
     </row>
-    <row r="95" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I95" s="14"/>
       <c r="J95" s="14"/>
     </row>
-    <row r="96" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I96" s="14"/>
       <c r="J96" s="14"/>
     </row>
-    <row r="97" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I97" s="14"/>
       <c r="J97" s="14"/>
     </row>
-    <row r="98" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I98" s="14"/>
       <c r="J98" s="14"/>
     </row>
-    <row r="99" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I99" s="14"/>
       <c r="J99" s="14"/>
     </row>
-    <row r="100" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I100" s="14"/>
       <c r="J100" s="14"/>
     </row>
-    <row r="101" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="101" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I101" s="14"/>
       <c r="J101" s="14"/>
     </row>
-    <row r="102" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="102" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I102" s="14"/>
       <c r="J102" s="14"/>
     </row>
-    <row r="103" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="103" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I103" s="14"/>
       <c r="J103" s="14"/>
     </row>
-    <row r="104" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="104" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I104" s="14"/>
       <c r="J104" s="14"/>
     </row>
-    <row r="105" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="105" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I105" s="14"/>
       <c r="J105" s="14"/>
     </row>
-    <row r="106" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="106" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I106" s="14"/>
       <c r="J106" s="14"/>
     </row>
-    <row r="107" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="107" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I107" s="14"/>
       <c r="J107" s="14"/>
     </row>
-    <row r="108" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="108" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I108" s="14"/>
       <c r="J108" s="14"/>
     </row>
-    <row r="109" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="109" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I109" s="14"/>
       <c r="J109" s="14"/>
     </row>
-    <row r="110" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="110" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I110" s="14"/>
       <c r="J110" s="14"/>
     </row>
-    <row r="111" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="111" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I111" s="14"/>
       <c r="J111" s="14"/>
     </row>
-    <row r="112" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="112" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I112" s="14"/>
       <c r="J112" s="14"/>
     </row>
-    <row r="113" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="113" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I113" s="14"/>
       <c r="J113" s="14"/>
     </row>
-    <row r="114" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="114" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I114" s="14"/>
       <c r="J114" s="14"/>
     </row>
-    <row r="115" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="115" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I115" s="14"/>
       <c r="J115" s="14"/>
     </row>
-    <row r="116" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="116" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I116" s="14"/>
       <c r="J116" s="14"/>
     </row>
-    <row r="117" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="117" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I117" s="14"/>
       <c r="J117" s="14"/>
     </row>
-    <row r="118" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="118" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I118" s="14"/>
       <c r="J118" s="14"/>
     </row>
-    <row r="119" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="119" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I119" s="14"/>
       <c r="J119" s="14"/>
     </row>
-    <row r="120" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="120" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I120" s="14"/>
       <c r="J120" s="14"/>
     </row>
-    <row r="121" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="121" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I121" s="14"/>
       <c r="J121" s="14"/>
     </row>
-    <row r="122" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="122" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I122" s="14"/>
       <c r="J122" s="14"/>
     </row>
-    <row r="123" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="123" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I123" s="14"/>
       <c r="J123" s="14"/>
     </row>
-    <row r="124" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="124" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I124" s="14"/>
       <c r="J124" s="14"/>
     </row>
-    <row r="125" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="125" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I125" s="14"/>
       <c r="J125" s="14"/>
     </row>
-    <row r="126" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="126" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I126" s="14"/>
       <c r="J126" s="14"/>
     </row>
-    <row r="127" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="127" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I127" s="14"/>
       <c r="J127" s="14"/>
     </row>
-    <row r="128" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="128" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I128" s="14"/>
       <c r="J128" s="14"/>
     </row>
-    <row r="129" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="129" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I129" s="14"/>
       <c r="J129" s="14"/>
     </row>
-    <row r="130" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="130" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I130" s="14"/>
       <c r="J130" s="14"/>
     </row>
-    <row r="131" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="131" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I131" s="14"/>
       <c r="J131" s="14"/>
     </row>
-    <row r="132" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="132" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I132" s="14"/>
       <c r="J132" s="14"/>
     </row>
-    <row r="133" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="133" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I133" s="14"/>
       <c r="J133" s="14"/>
     </row>
-    <row r="134" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="134" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I134" s="14"/>
       <c r="J134" s="14"/>
     </row>
-    <row r="135" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="135" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I135" s="14"/>
       <c r="J135" s="14"/>
     </row>
-    <row r="136" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="136" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I136" s="14"/>
       <c r="J136" s="14"/>
     </row>
-    <row r="137" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="137" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I137" s="14"/>
       <c r="J137" s="14"/>
     </row>
-    <row r="138" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="138" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I138" s="14"/>
       <c r="J138" s="14"/>
     </row>
-    <row r="139" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="139" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I139" s="14"/>
       <c r="J139" s="14"/>
     </row>
-    <row r="140" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="140" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I140" s="14"/>
       <c r="J140" s="14"/>
     </row>
-    <row r="141" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="141" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I141" s="14"/>
       <c r="J141" s="14"/>
     </row>
-    <row r="142" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="142" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I142" s="14"/>
       <c r="J142" s="14"/>
     </row>
-    <row r="143" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="143" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I143" s="14"/>
       <c r="J143" s="14"/>
     </row>
-    <row r="144" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="144" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I144" s="14"/>
       <c r="J144" s="14"/>
     </row>
-    <row r="145" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="145" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I145" s="14"/>
       <c r="J145" s="14"/>
     </row>
-    <row r="146" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="146" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I146" s="14"/>
       <c r="J146" s="14"/>
     </row>
-    <row r="147" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="147" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I147" s="14"/>
       <c r="J147" s="14"/>
     </row>
-    <row r="148" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="148" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I148" s="14"/>
       <c r="J148" s="14"/>
     </row>
-    <row r="149" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="149" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I149" s="14"/>
       <c r="J149" s="14"/>
     </row>
-    <row r="150" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="150" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I150" s="14"/>
       <c r="J150" s="14"/>
     </row>
-    <row r="151" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="151" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I151" s="14"/>
       <c r="J151" s="14"/>
     </row>
-    <row r="152" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="152" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I152" s="14"/>
       <c r="J152" s="14"/>
     </row>
-    <row r="153" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="153" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I153" s="14"/>
       <c r="J153" s="14"/>
     </row>
-    <row r="154" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="154" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I154" s="14"/>
       <c r="J154" s="14"/>
     </row>
-    <row r="155" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="155" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I155" s="14"/>
       <c r="J155" s="14"/>
     </row>
-    <row r="156" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="156" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I156" s="14"/>
       <c r="J156" s="14"/>
     </row>
-    <row r="157" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="157" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I157" s="14"/>
       <c r="J157" s="14"/>
     </row>
-    <row r="158" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="158" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I158" s="14"/>
       <c r="J158" s="14"/>
     </row>
-    <row r="159" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="159" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I159" s="14"/>
       <c r="J159" s="14"/>
     </row>
-    <row r="160" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="160" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I160" s="14"/>
       <c r="J160" s="14"/>
     </row>
-    <row r="161" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="161" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I161" s="14"/>
       <c r="J161" s="14"/>
     </row>
-    <row r="162" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="162" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I162" s="14"/>
       <c r="J162" s="14"/>
     </row>
-    <row r="163" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="163" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I163" s="14"/>
       <c r="J163" s="14"/>
     </row>
-    <row r="164" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="164" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I164" s="14"/>
       <c r="J164" s="14"/>
     </row>
-    <row r="165" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="165" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I165" s="14"/>
       <c r="J165" s="14"/>
     </row>
-    <row r="166" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="166" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I166" s="14"/>
       <c r="J166" s="14"/>
     </row>
-    <row r="167" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="167" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I167" s="14"/>
       <c r="J167" s="14"/>
     </row>
-    <row r="168" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="168" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I168" s="14"/>
       <c r="J168" s="14"/>
     </row>
-    <row r="169" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="169" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I169" s="14"/>
       <c r="J169" s="14"/>
     </row>
-    <row r="170" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="170" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I170" s="14"/>
       <c r="J170" s="14"/>
     </row>
-    <row r="171" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="171" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I171" s="14"/>
       <c r="J171" s="14"/>
     </row>
-    <row r="172" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="172" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I172" s="14"/>
       <c r="J172" s="14"/>
     </row>
-    <row r="173" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="173" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I173" s="14"/>
       <c r="J173" s="14"/>
     </row>
-    <row r="174" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="174" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I174" s="14"/>
       <c r="J174" s="14"/>
     </row>
-    <row r="175" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="175" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I175" s="14"/>
       <c r="J175" s="14"/>
     </row>
-    <row r="176" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="176" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I176" s="14"/>
       <c r="J176" s="14"/>
     </row>
-    <row r="177" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="177" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I177" s="14"/>
       <c r="J177" s="14"/>
     </row>
-    <row r="178" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="178" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I178" s="14"/>
       <c r="J178" s="14"/>
     </row>
-    <row r="179" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="179" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I179" s="14"/>
       <c r="J179" s="14"/>
     </row>
-    <row r="180" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="180" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I180" s="14"/>
       <c r="J180" s="14"/>
     </row>
-    <row r="181" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="181" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I181" s="14"/>
       <c r="J181" s="14"/>
     </row>
-    <row r="182" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="182" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I182" s="14"/>
       <c r="J182" s="14"/>
     </row>
-    <row r="183" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="183" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I183" s="14"/>
       <c r="J183" s="14"/>
     </row>
-    <row r="184" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="184" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I184" s="14"/>
       <c r="J184" s="14"/>
     </row>
-    <row r="185" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="185" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I185" s="14"/>
       <c r="J185" s="14"/>
     </row>
-    <row r="186" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="186" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I186" s="14"/>
       <c r="J186" s="14"/>
     </row>
-    <row r="187" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="187" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I187" s="14"/>
       <c r="J187" s="14"/>
     </row>
-    <row r="188" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="188" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I188" s="14"/>
       <c r="J188" s="14"/>
     </row>
-    <row r="189" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="189" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I189" s="14"/>
       <c r="J189" s="14"/>
     </row>
-    <row r="190" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="190" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I190" s="14"/>
       <c r="J190" s="14"/>
     </row>
-    <row r="191" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="191" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I191" s="14"/>
       <c r="J191" s="14"/>
     </row>
-    <row r="192" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="192" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I192" s="14"/>
       <c r="J192" s="14"/>
     </row>
-    <row r="193" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="193" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I193" s="14"/>
       <c r="J193" s="14"/>
     </row>
-    <row r="194" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="194" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I194" s="14"/>
       <c r="J194" s="14"/>
     </row>
-    <row r="195" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="195" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I195" s="14"/>
       <c r="J195" s="14"/>
     </row>
-    <row r="196" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="196" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I196" s="14"/>
       <c r="J196" s="14"/>
     </row>
-    <row r="197" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="197" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I197" s="14"/>
       <c r="J197" s="14"/>
     </row>
-    <row r="198" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="198" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I198" s="14"/>
       <c r="J198" s="14"/>
     </row>
-    <row r="199" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="199" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I199" s="14"/>
       <c r="J199" s="14"/>
     </row>
-    <row r="200" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="200" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I200" s="14"/>
       <c r="J200" s="14"/>
     </row>
-    <row r="201" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="201" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I201" s="14"/>
       <c r="J201" s="14"/>
     </row>
-    <row r="202" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="202" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I202" s="14"/>
       <c r="J202" s="14"/>
     </row>
-    <row r="203" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="203" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I203" s="14"/>
       <c r="J203" s="14"/>
     </row>
-    <row r="204" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="204" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I204" s="14"/>
       <c r="J204" s="14"/>
     </row>
-    <row r="205" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="205" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I205" s="14"/>
       <c r="J205" s="14"/>
     </row>
-    <row r="206" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="206" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I206" s="14"/>
       <c r="J206" s="14"/>
     </row>
-    <row r="207" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="207" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I207" s="14"/>
       <c r="J207" s="14"/>
     </row>
-    <row r="208" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="208" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I208" s="14"/>
       <c r="J208" s="14"/>
     </row>
-    <row r="209" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="209" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I209" s="14"/>
       <c r="J209" s="14"/>
     </row>
-    <row r="210" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="210" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I210" s="14"/>
       <c r="J210" s="14"/>
     </row>
-    <row r="211" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="211" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I211" s="14"/>
       <c r="J211" s="14"/>
     </row>
-    <row r="212" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="212" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I212" s="14"/>
       <c r="J212" s="14"/>
     </row>
-    <row r="213" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="213" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I213" s="14"/>
       <c r="J213" s="14"/>
     </row>
-    <row r="214" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="214" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I214" s="14"/>
       <c r="J214" s="14"/>
     </row>
-    <row r="215" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="215" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I215" s="14"/>
       <c r="J215" s="14"/>
     </row>
-    <row r="216" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="216" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I216" s="14"/>
       <c r="J216" s="14"/>
     </row>
-    <row r="217" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="217" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I217" s="14"/>
       <c r="J217" s="14"/>
     </row>
-    <row r="218" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="218" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I218" s="14"/>
       <c r="J218" s="14"/>
     </row>
-    <row r="219" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="219" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I219" s="14"/>
       <c r="J219" s="14"/>
     </row>
-    <row r="220" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="220" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I220" s="14"/>
       <c r="J220" s="14"/>
     </row>
-    <row r="221" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="221" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I221" s="14"/>
       <c r="J221" s="14"/>
     </row>
-    <row r="222" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="222" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I222" s="14"/>
       <c r="J222" s="14"/>
     </row>
-    <row r="223" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="223" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I223" s="14"/>
       <c r="J223" s="14"/>
     </row>
-    <row r="224" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="224" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I224" s="14"/>
       <c r="J224" s="14"/>
     </row>
-    <row r="225" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="225" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I225" s="14"/>
       <c r="J225" s="14"/>
     </row>
-    <row r="226" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="226" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I226" s="14"/>
       <c r="J226" s="14"/>
     </row>
-    <row r="227" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="227" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I227" s="14"/>
       <c r="J227" s="14"/>
     </row>
-    <row r="228" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="228" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I228" s="14"/>
       <c r="J228" s="14"/>
     </row>
-    <row r="229" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="229" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I229" s="14"/>
       <c r="J229" s="14"/>
     </row>
-    <row r="230" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="230" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I230" s="14"/>
       <c r="J230" s="14"/>
     </row>
-    <row r="231" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="231" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I231" s="14"/>
       <c r="J231" s="14"/>
     </row>
-    <row r="232" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="232" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I232" s="14"/>
       <c r="J232" s="14"/>
     </row>
-    <row r="233" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="233" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I233" s="14"/>
       <c r="J233" s="14"/>
     </row>
-    <row r="234" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="234" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I234" s="14"/>
       <c r="J234" s="14"/>
     </row>
-    <row r="235" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="235" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I235" s="14"/>
       <c r="J235" s="14"/>
     </row>
-    <row r="236" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="236" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I236" s="14"/>
       <c r="J236" s="14"/>
     </row>
-    <row r="237" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="237" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I237" s="14"/>
       <c r="J237" s="14"/>
     </row>
-    <row r="238" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="238" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I238" s="14"/>
       <c r="J238" s="14"/>
     </row>
-    <row r="239" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="239" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I239" s="14"/>
       <c r="J239" s="14"/>
     </row>
-    <row r="240" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="240" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I240" s="14"/>
       <c r="J240" s="14"/>
     </row>
-    <row r="241" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="241" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I241" s="14"/>
       <c r="J241" s="14"/>
     </row>
-    <row r="242" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="242" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I242" s="14"/>
       <c r="J242" s="14"/>
     </row>
-    <row r="243" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="243" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I243" s="14"/>
       <c r="J243" s="14"/>
     </row>
-    <row r="244" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="244" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I244" s="14"/>
       <c r="J244" s="14"/>
     </row>
-    <row r="245" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="245" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I245" s="14"/>
       <c r="J245" s="14"/>
     </row>
-    <row r="246" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="246" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I246" s="14"/>
       <c r="J246" s="14"/>
     </row>
-    <row r="247" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="247" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I247" s="14"/>
       <c r="J247" s="14"/>
     </row>
-    <row r="248" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="248" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I248" s="14"/>
       <c r="J248" s="14"/>
     </row>
-    <row r="249" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="249" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I249" s="14"/>
       <c r="J249" s="14"/>
     </row>
-    <row r="250" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="250" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I250" s="14"/>
       <c r="J250" s="14"/>
     </row>
-    <row r="251" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="251" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I251" s="14"/>
       <c r="J251" s="14"/>
     </row>
-    <row r="252" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="252" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I252" s="14"/>
       <c r="J252" s="14"/>
     </row>
-    <row r="253" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="253" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I253" s="14"/>
       <c r="J253" s="14"/>
     </row>
-    <row r="254" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="254" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I254" s="14"/>
       <c r="J254" s="14"/>
     </row>
-    <row r="255" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="255" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I255" s="14"/>
       <c r="J255" s="14"/>
     </row>
-    <row r="256" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="256" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I256" s="14"/>
       <c r="J256" s="14"/>
     </row>
-    <row r="257" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="257" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I257" s="14"/>
       <c r="J257" s="14"/>
     </row>
-    <row r="258" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="258" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I258" s="14"/>
       <c r="J258" s="14"/>
     </row>
-    <row r="259" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="259" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I259" s="14"/>
       <c r="J259" s="14"/>
     </row>
-    <row r="260" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="260" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I260" s="14"/>
       <c r="J260" s="14"/>
     </row>
-    <row r="261" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="261" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I261" s="14"/>
       <c r="J261" s="14"/>
     </row>
-    <row r="262" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="262" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I262" s="14"/>
       <c r="J262" s="14"/>
     </row>
-    <row r="263" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="263" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I263" s="14"/>
       <c r="J263" s="14"/>
     </row>
-    <row r="264" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="264" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I264" s="14"/>
       <c r="J264" s="14"/>
     </row>
-    <row r="265" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="265" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I265" s="14"/>
       <c r="J265" s="14"/>
     </row>
-    <row r="266" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="266" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I266" s="14"/>
       <c r="J266" s="14"/>
     </row>
-    <row r="267" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="267" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I267" s="14"/>
       <c r="J267" s="14"/>
     </row>
-    <row r="268" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="268" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I268" s="14"/>
       <c r="J268" s="14"/>
     </row>
-    <row r="269" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="269" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I269" s="14"/>
       <c r="J269" s="14"/>
     </row>
-    <row r="270" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="270" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I270" s="14"/>
       <c r="J270" s="14"/>
     </row>
-    <row r="271" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="271" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I271" s="14"/>
       <c r="J271" s="14"/>
     </row>
-    <row r="272" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="272" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I272" s="14"/>
       <c r="J272" s="14"/>
     </row>
-    <row r="273" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="273" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I273" s="14"/>
       <c r="J273" s="14"/>
     </row>
-    <row r="274" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="274" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I274" s="14"/>
       <c r="J274" s="14"/>
     </row>
-    <row r="275" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="275" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I275" s="14"/>
       <c r="J275" s="14"/>
     </row>
-    <row r="276" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="276" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I276" s="14"/>
       <c r="J276" s="14"/>
     </row>
-    <row r="277" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="277" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I277" s="14"/>
       <c r="J277" s="14"/>
     </row>
-    <row r="278" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="278" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I278" s="14"/>
       <c r="J278" s="14"/>
     </row>
-    <row r="279" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="279" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I279" s="14"/>
       <c r="J279" s="14"/>
     </row>
-    <row r="280" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="280" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I280" s="14"/>
       <c r="J280" s="14"/>
     </row>
-    <row r="281" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="281" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I281" s="14"/>
       <c r="J281" s="14"/>
     </row>
-    <row r="282" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="282" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I282" s="14"/>
       <c r="J282" s="14"/>
     </row>
-    <row r="283" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="283" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I283" s="14"/>
       <c r="J283" s="14"/>
     </row>
-    <row r="284" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="284" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I284" s="14"/>
       <c r="J284" s="14"/>
     </row>
-    <row r="285" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="285" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I285" s="14"/>
       <c r="J285" s="14"/>
     </row>
-    <row r="286" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="286" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I286" s="14"/>
       <c r="J286" s="14"/>
     </row>
-    <row r="287" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="287" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I287" s="14"/>
       <c r="J287" s="14"/>
     </row>
-    <row r="288" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="288" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I288" s="14"/>
       <c r="J288" s="14"/>
     </row>
-    <row r="289" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="289" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I289" s="14"/>
       <c r="J289" s="14"/>
     </row>
-    <row r="290" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="290" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I290" s="14"/>
       <c r="J290" s="14"/>
     </row>
-    <row r="291" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="291" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I291" s="14"/>
       <c r="J291" s="14"/>
     </row>
-    <row r="292" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="292" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I292" s="14"/>
       <c r="J292" s="14"/>
     </row>
-    <row r="293" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="293" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I293" s="14"/>
       <c r="J293" s="14"/>
     </row>
-    <row r="294" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="294" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I294" s="14"/>
       <c r="J294" s="14"/>
     </row>
-    <row r="295" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="295" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I295" s="14"/>
       <c r="J295" s="14"/>
     </row>
-    <row r="296" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="296" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I296" s="14"/>
       <c r="J296" s="14"/>
     </row>
-    <row r="297" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="297" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I297" s="14"/>
       <c r="J297" s="14"/>
     </row>
-    <row r="298" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="298" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I298" s="14"/>
       <c r="J298" s="14"/>
     </row>
-    <row r="299" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="299" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I299" s="14"/>
       <c r="J299" s="14"/>
     </row>
-    <row r="300" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="300" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I300" s="14"/>
       <c r="J300" s="14"/>
     </row>
-    <row r="301" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="301" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I301" s="14"/>
       <c r="J301" s="14"/>
     </row>
-    <row r="302" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="302" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I302" s="14"/>
       <c r="J302" s="14"/>
     </row>
-    <row r="303" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="303" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I303" s="14"/>
       <c r="J303" s="14"/>
     </row>
-    <row r="304" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="304" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I304" s="14"/>
       <c r="J304" s="14"/>
     </row>
-    <row r="305" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="305" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I305" s="14"/>
       <c r="J305" s="14"/>
     </row>
-    <row r="306" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="306" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I306" s="14"/>
       <c r="J306" s="14"/>
     </row>
-    <row r="307" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="307" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I307" s="14"/>
       <c r="J307" s="14"/>
     </row>
-    <row r="308" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="308" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I308" s="14"/>
       <c r="J308" s="14"/>
     </row>
-    <row r="309" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="309" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I309" s="14"/>
       <c r="J309" s="14"/>
     </row>
-    <row r="310" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="310" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I310" s="14"/>
       <c r="J310" s="14"/>
     </row>
-    <row r="311" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="311" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I311" s="14"/>
       <c r="J311" s="14"/>
     </row>
-    <row r="312" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="312" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I312" s="14"/>
       <c r="J312" s="14"/>
     </row>
-    <row r="313" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="313" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I313" s="14"/>
       <c r="J313" s="14"/>
     </row>
-    <row r="314" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="314" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I314" s="14"/>
       <c r="J314" s="14"/>
     </row>
-    <row r="315" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="315" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I315" s="14"/>
       <c r="J315" s="14"/>
     </row>
-    <row r="316" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="316" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I316" s="14"/>
       <c r="J316" s="14"/>
     </row>
-    <row r="317" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="317" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I317" s="14"/>
       <c r="J317" s="14"/>
     </row>
-    <row r="318" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="318" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I318" s="14"/>
       <c r="J318" s="14"/>
     </row>
-    <row r="319" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="319" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I319" s="14"/>
       <c r="J319" s="14"/>
     </row>
-    <row r="320" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="320" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I320" s="14"/>
       <c r="J320" s="14"/>
     </row>
-    <row r="321" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="321" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I321" s="14"/>
       <c r="J321" s="14"/>
     </row>
-    <row r="322" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="322" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I322" s="14"/>
       <c r="J322" s="14"/>
     </row>
-    <row r="323" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="323" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I323" s="14"/>
       <c r="J323" s="14"/>
     </row>
-    <row r="324" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="324" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I324" s="14"/>
       <c r="J324" s="14"/>
     </row>
-    <row r="325" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="325" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I325" s="14"/>
       <c r="J325" s="14"/>
     </row>
-    <row r="326" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="326" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I326" s="14"/>
       <c r="J326" s="14"/>
     </row>
-    <row r="327" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="327" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I327" s="14"/>
       <c r="J327" s="14"/>
     </row>
-    <row r="328" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="328" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I328" s="14"/>
       <c r="J328" s="14"/>
     </row>
-    <row r="329" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="329" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I329" s="14"/>
       <c r="J329" s="14"/>
     </row>
-    <row r="330" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="330" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I330" s="14"/>
       <c r="J330" s="14"/>
     </row>
-    <row r="331" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="331" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I331" s="14"/>
       <c r="J331" s="14"/>
     </row>
-    <row r="332" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="332" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I332" s="14"/>
       <c r="J332" s="14"/>
     </row>
-    <row r="333" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="333" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I333" s="14"/>
       <c r="J333" s="14"/>
     </row>
-    <row r="334" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="334" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I334" s="14"/>
       <c r="J334" s="14"/>
     </row>
-    <row r="335" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="335" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I335" s="14"/>
       <c r="J335" s="14"/>
     </row>
-    <row r="336" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="336" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I336" s="14"/>
       <c r="J336" s="14"/>
     </row>
-    <row r="337" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="337" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I337" s="14"/>
       <c r="J337" s="14"/>
     </row>
-    <row r="338" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="338" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I338" s="14"/>
       <c r="J338" s="14"/>
     </row>
-    <row r="339" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="339" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I339" s="14"/>
       <c r="J339" s="14"/>
     </row>
-    <row r="340" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="340" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I340" s="14"/>
       <c r="J340" s="14"/>
     </row>
-    <row r="341" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="341" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I341" s="14"/>
       <c r="J341" s="14"/>
     </row>
-    <row r="342" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="342" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I342" s="14"/>
       <c r="J342" s="14"/>
     </row>
-    <row r="343" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="343" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I343" s="14"/>
       <c r="J343" s="14"/>
     </row>
-    <row r="344" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="344" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I344" s="14"/>
       <c r="J344" s="14"/>
     </row>
-    <row r="345" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="345" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I345" s="14"/>
       <c r="J345" s="14"/>
     </row>
-    <row r="346" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="346" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I346" s="14"/>
       <c r="J346" s="14"/>
     </row>
-    <row r="347" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="347" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I347" s="14"/>
       <c r="J347" s="14"/>
     </row>
-    <row r="348" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="348" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I348" s="14"/>
       <c r="J348" s="14"/>
     </row>
-    <row r="349" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="349" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I349" s="14"/>
       <c r="J349" s="14"/>
     </row>
-    <row r="350" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="350" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I350" s="14"/>
       <c r="J350" s="14"/>
     </row>
-    <row r="351" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="351" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I351" s="14"/>
       <c r="J351" s="14"/>
     </row>
-    <row r="352" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="352" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I352" s="14"/>
       <c r="J352" s="14"/>
     </row>
@@ -2838,23 +2827,23 @@
   </sheetPr>
   <dimension ref="A1:AY47"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD29"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9.109375" style="1"/>
-    <col min="3" max="7" width="9.109375" style="4"/>
-    <col min="8" max="10" width="9.109375" style="1"/>
-    <col min="11" max="11" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="7" width="9.140625" style="4"/>
+    <col min="8" max="10" width="9.140625" style="1"/>
+    <col min="11" max="11" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>55</v>
       </c>
@@ -2903,7 +2892,7 @@
       <c r="AG1" s="9"/>
       <c r="AH1" s="6"/>
     </row>
-    <row r="2" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>2E-3</v>
       </c>
@@ -2935,7 +2924,7 @@
         <v>1E-4</v>
       </c>
       <c r="K2" s="7">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="L2" s="7">
         <f>1/10</f>
@@ -2955,7 +2944,7 @@
       <c r="AG2" s="6"/>
       <c r="AH2" s="6"/>
     </row>
-    <row r="3" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F3" s="12"/>
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
@@ -2996,7 +2985,7 @@
       <c r="AX3" s="6"/>
       <c r="AY3" s="6"/>
     </row>
-    <row r="4" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F4" s="12"/>
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
@@ -3037,7 +3026,7 @@
       <c r="AX4" s="6"/>
       <c r="AY4" s="6"/>
     </row>
-    <row r="5" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F5" s="12"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
@@ -3078,7 +3067,7 @@
       <c r="AX5" s="6"/>
       <c r="AY5" s="6"/>
     </row>
-    <row r="6" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -3119,7 +3108,7 @@
       <c r="AX6" s="6"/>
       <c r="AY6" s="6"/>
     </row>
-    <row r="7" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
@@ -3160,7 +3149,7 @@
       <c r="AX7" s="6"/>
       <c r="AY7" s="6"/>
     </row>
-    <row r="8" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F8" s="12"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
@@ -3201,7 +3190,7 @@
       <c r="AX8" s="6"/>
       <c r="AY8" s="6"/>
     </row>
-    <row r="9" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
@@ -3242,7 +3231,7 @@
       <c r="AX9" s="6"/>
       <c r="AY9" s="6"/>
     </row>
-    <row r="10" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F10" s="12"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
@@ -3283,7 +3272,7 @@
       <c r="AX10" s="6"/>
       <c r="AY10" s="6"/>
     </row>
-    <row r="11" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F11" s="12"/>
       <c r="I11" s="12"/>
       <c r="J11" s="12"/>
@@ -3324,7 +3313,7 @@
       <c r="AX11" s="6"/>
       <c r="AY11" s="6"/>
     </row>
-    <row r="12" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F12" s="12"/>
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
@@ -3365,7 +3354,7 @@
       <c r="AX12" s="6"/>
       <c r="AY12" s="6"/>
     </row>
-    <row r="13" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F13" s="12"/>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
@@ -3406,7 +3395,7 @@
       <c r="AX13" s="6"/>
       <c r="AY13" s="6"/>
     </row>
-    <row r="14" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F14" s="12"/>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
@@ -3447,7 +3436,7 @@
       <c r="AX14" s="6"/>
       <c r="AY14" s="6"/>
     </row>
-    <row r="15" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F15" s="12"/>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
@@ -3488,7 +3477,7 @@
       <c r="AX15" s="6"/>
       <c r="AY15" s="6"/>
     </row>
-    <row r="16" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F16" s="12"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
@@ -3529,7 +3518,7 @@
       <c r="AX16" s="6"/>
       <c r="AY16" s="6"/>
     </row>
-    <row r="17" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F17" s="12"/>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
@@ -3570,7 +3559,7 @@
       <c r="AX17" s="6"/>
       <c r="AY17" s="6"/>
     </row>
-    <row r="18" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F18" s="12"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
@@ -3611,90 +3600,90 @@
       <c r="AX18" s="6"/>
       <c r="AY18" s="6"/>
     </row>
-    <row r="19" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F19" s="12"/>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
       <c r="M19" s="13"/>
     </row>
-    <row r="20" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F20" s="12"/>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
       <c r="M20" s="13"/>
     </row>
-    <row r="21" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F21" s="12"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
       <c r="M21" s="13"/>
     </row>
-    <row r="22" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F22" s="12"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
       <c r="M22" s="13"/>
     </row>
-    <row r="23" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F23" s="12"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
       <c r="M23" s="13"/>
     </row>
-    <row r="24" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F24" s="12"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
       <c r="M24" s="13"/>
     </row>
-    <row r="25" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F25" s="12"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
       <c r="M25" s="13"/>
     </row>
-    <row r="26" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F26" s="12"/>
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
       <c r="M26" s="13"/>
     </row>
-    <row r="27" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F27" s="12"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
       <c r="M27" s="13"/>
     </row>
-    <row r="28" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F28" s="12"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
       <c r="M28" s="13"/>
     </row>
-    <row r="29" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F29" s="12"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
       <c r="M29" s="13"/>
     </row>
-    <row r="30" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3711,13 +3700,13 @@
   </sheetPr>
   <dimension ref="A1:AE1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+    <sheetView zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:31" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
@@ -3825,9 +3814,9 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:30" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
add sheet with GFOR test PLL
</commit_message>
<xml_diff>
--- a/stability_analysis/data/cases/IEEE_118_FULL_data_vsc.xlsx
+++ b/stability_analysis/data/cases/IEEE_118_FULL_data_vsc.xlsx
@@ -1,41 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francesca\miniconda3\envs\gridcal_original\stability_analysis\stability_analysis\data\cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francesca\miniconda3\envs\gridcal_original2\stability_analysis\stability_analysis\data\cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6BDDA17-991F-4761-A5B4-97D80320A1C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A50236-72F7-4A94-B9E6-2C091AC92851}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="922" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" tabRatio="922" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STATCOM" sheetId="4" r:id="rId1"/>
-    <sheet name="UserGFOL" sheetId="19" r:id="rId2"/>
-    <sheet name="UserGFOR" sheetId="20" r:id="rId3"/>
-    <sheet name="MMC-Pac-GFll" sheetId="21" r:id="rId4"/>
-    <sheet name="MMC-Vdc-GFll" sheetId="22" r:id="rId5"/>
+    <sheet name="UserGFOL" sheetId="23" r:id="rId2"/>
+    <sheet name="UserGFOL_test" sheetId="19" r:id="rId3"/>
+    <sheet name="UserGFOR" sheetId="20" r:id="rId4"/>
+    <sheet name="MMC-Pac-GFll" sheetId="21" r:id="rId5"/>
+    <sheet name="MMC-Vdc-GFll" sheetId="22" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="61">
   <si>
     <t>bus</t>
   </si>
@@ -657,14 +647,14 @@
       <selection activeCell="G16" sqref="G15:G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="6.6640625" style="4" customWidth="1"/>
-    <col min="3" max="52" width="6.6640625" style="1" customWidth="1"/>
-    <col min="53" max="16384" width="8.6640625" style="1"/>
+    <col min="1" max="2" width="6.7109375" style="4" customWidth="1"/>
+    <col min="3" max="52" width="6.7109375" style="1" customWidth="1"/>
+    <col min="53" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -757,7 +747,7 @@
       <c r="AX1" s="6"/>
       <c r="AY1" s="6"/>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:51" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -809,7 +799,7 @@
       <c r="AX2" s="2"/>
       <c r="AY2" s="2"/>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="2"/>
@@ -862,7 +852,7 @@
       <c r="AX3" s="2"/>
       <c r="AY3" s="2"/>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -915,7 +905,7 @@
       <c r="AX4" s="2"/>
       <c r="AY4" s="2"/>
     </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="8"/>
@@ -979,32 +969,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E10B533E-38A2-4A18-91F9-81A95CC6AC6B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7AADD0-B5C3-4B33-83C3-7F96BC1AEB8D}">
   <sheetPr>
     <tabColor theme="0" tint="-0.14999847407452621"/>
   </sheetPr>
   <dimension ref="A1:AF352"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="6.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.6640625" style="1" customWidth="1"/>
-    <col min="9" max="10" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="5" width="6.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" style="1" customWidth="1"/>
+    <col min="9" max="10" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="50" width="6.6640625" style="1" customWidth="1"/>
-    <col min="51" max="16384" width="8.6640625" style="1"/>
+    <col min="14" max="14" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="50" width="6.7109375" style="1" customWidth="1"/>
+    <col min="51" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>55</v>
       </c>
@@ -1059,7 +1049,7 @@
       <c r="AE1" s="8"/>
       <c r="AF1" s="2"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>2E-3</v>
       </c>
@@ -1109,7 +1099,7 @@
       <c r="AE2" s="2"/>
       <c r="AF2" s="2"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -1125,7 +1115,7 @@
       <c r="M3" s="16"/>
       <c r="N3" s="7"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -1141,7 +1131,7 @@
       <c r="M4" s="16"/>
       <c r="N4" s="7"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -1157,7 +1147,7 @@
       <c r="M5" s="16"/>
       <c r="N5" s="7"/>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -1173,7 +1163,7 @@
       <c r="M6" s="16"/>
       <c r="N6" s="7"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1189,7 +1179,7 @@
       <c r="M7" s="16"/>
       <c r="N7" s="7"/>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -1205,7 +1195,7 @@
       <c r="M8" s="16"/>
       <c r="N8" s="7"/>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1221,7 +1211,7 @@
       <c r="M9" s="16"/>
       <c r="N9" s="7"/>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1237,7 +1227,7 @@
       <c r="M10" s="16"/>
       <c r="N10" s="7"/>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -1253,7 +1243,7 @@
       <c r="M11" s="16"/>
       <c r="N11" s="7"/>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -1269,7 +1259,7 @@
       <c r="M12" s="16"/>
       <c r="N12" s="7"/>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -1285,7 +1275,7 @@
       <c r="M13" s="16"/>
       <c r="N13" s="7"/>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -1301,7 +1291,7 @@
       <c r="M14" s="16"/>
       <c r="N14" s="7"/>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -1317,7 +1307,7 @@
       <c r="M15" s="16"/>
       <c r="N15" s="7"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -1333,7 +1323,7 @@
       <c r="M16" s="16"/>
       <c r="N16" s="7"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -1349,7 +1339,7 @@
       <c r="M17" s="16"/>
       <c r="N17" s="7"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -1365,7 +1355,7 @@
       <c r="M18" s="16"/>
       <c r="N18" s="7"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -1381,7 +1371,7 @@
       <c r="M19" s="16"/>
       <c r="N19" s="7"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -1397,7 +1387,7 @@
       <c r="M20" s="16"/>
       <c r="N20" s="7"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -1413,7 +1403,7 @@
       <c r="M21" s="16"/>
       <c r="N21" s="7"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -1429,7 +1419,7 @@
       <c r="M22" s="16"/>
       <c r="N22" s="7"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -1445,7 +1435,7 @@
       <c r="M23" s="16"/>
       <c r="N23" s="7"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -1461,7 +1451,7 @@
       <c r="M24" s="16"/>
       <c r="N24" s="7"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -1477,7 +1467,7 @@
       <c r="M25" s="16"/>
       <c r="N25" s="7"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -1493,7 +1483,7 @@
       <c r="M26" s="16"/>
       <c r="N26" s="7"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -1509,7 +1499,7 @@
       <c r="M27" s="16"/>
       <c r="N27" s="7"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -1525,1299 +1515,1299 @@
       <c r="M28" s="16"/>
       <c r="N28" s="7"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="I29" s="14"/>
       <c r="J29" s="14"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="I30" s="14"/>
       <c r="J30" s="14"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="I31" s="14"/>
       <c r="J31" s="14"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="I32" s="14"/>
       <c r="J32" s="14"/>
     </row>
-    <row r="33" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I33" s="14"/>
       <c r="J33" s="14"/>
     </row>
-    <row r="34" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I34" s="14"/>
       <c r="J34" s="14"/>
     </row>
-    <row r="35" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I35" s="14"/>
       <c r="J35" s="14"/>
     </row>
-    <row r="36" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I36" s="14"/>
       <c r="J36" s="14"/>
     </row>
-    <row r="37" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I37" s="14"/>
       <c r="J37" s="14"/>
     </row>
-    <row r="38" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I38" s="14"/>
       <c r="J38" s="14"/>
     </row>
-    <row r="39" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I39" s="14"/>
       <c r="J39" s="14"/>
     </row>
-    <row r="40" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I40" s="14"/>
       <c r="J40" s="14"/>
     </row>
-    <row r="41" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I41" s="14"/>
       <c r="J41" s="14"/>
     </row>
-    <row r="42" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I42" s="14"/>
       <c r="J42" s="14"/>
     </row>
-    <row r="43" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I43" s="14"/>
       <c r="J43" s="14"/>
     </row>
-    <row r="44" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I44" s="14"/>
       <c r="J44" s="14"/>
     </row>
-    <row r="45" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I45" s="14"/>
       <c r="J45" s="14"/>
     </row>
-    <row r="46" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I46" s="14"/>
       <c r="J46" s="14"/>
     </row>
-    <row r="47" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I47" s="14"/>
       <c r="J47" s="14"/>
     </row>
-    <row r="48" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I48" s="14"/>
       <c r="J48" s="14"/>
     </row>
-    <row r="49" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I49" s="14"/>
       <c r="J49" s="14"/>
     </row>
-    <row r="50" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I50" s="14"/>
       <c r="J50" s="14"/>
     </row>
-    <row r="51" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I51" s="14"/>
       <c r="J51" s="14"/>
     </row>
-    <row r="52" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I52" s="14"/>
       <c r="J52" s="14"/>
     </row>
-    <row r="53" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I53" s="14"/>
       <c r="J53" s="14"/>
     </row>
-    <row r="54" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I54" s="14"/>
       <c r="J54" s="14"/>
     </row>
-    <row r="55" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I55" s="14"/>
       <c r="J55" s="14"/>
     </row>
-    <row r="56" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I56" s="14"/>
       <c r="J56" s="14"/>
     </row>
-    <row r="57" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I57" s="14"/>
       <c r="J57" s="14"/>
     </row>
-    <row r="58" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I58" s="14"/>
       <c r="J58" s="14"/>
     </row>
-    <row r="59" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I59" s="14"/>
       <c r="J59" s="14"/>
     </row>
-    <row r="60" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I60" s="14"/>
       <c r="J60" s="14"/>
     </row>
-    <row r="61" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I61" s="14"/>
       <c r="J61" s="14"/>
     </row>
-    <row r="62" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I62" s="14"/>
       <c r="J62" s="14"/>
     </row>
-    <row r="63" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I63" s="14"/>
       <c r="J63" s="14"/>
     </row>
-    <row r="64" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I64" s="14"/>
       <c r="J64" s="14"/>
     </row>
-    <row r="65" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I65" s="14"/>
       <c r="J65" s="14"/>
     </row>
-    <row r="66" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I66" s="14"/>
       <c r="J66" s="14"/>
     </row>
-    <row r="67" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I67" s="14"/>
       <c r="J67" s="14"/>
     </row>
-    <row r="68" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I68" s="14"/>
       <c r="J68" s="14"/>
     </row>
-    <row r="69" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I69" s="14"/>
       <c r="J69" s="14"/>
     </row>
-    <row r="70" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I70" s="14"/>
       <c r="J70" s="14"/>
     </row>
-    <row r="71" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I71" s="14"/>
       <c r="J71" s="14"/>
     </row>
-    <row r="72" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I72" s="14"/>
       <c r="J72" s="14"/>
     </row>
-    <row r="73" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I73" s="14"/>
       <c r="J73" s="14"/>
     </row>
-    <row r="74" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I74" s="14"/>
       <c r="J74" s="14"/>
     </row>
-    <row r="75" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I75" s="14"/>
       <c r="J75" s="14"/>
     </row>
-    <row r="76" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I76" s="14"/>
       <c r="J76" s="14"/>
     </row>
-    <row r="77" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I77" s="14"/>
       <c r="J77" s="14"/>
     </row>
-    <row r="78" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I78" s="14"/>
       <c r="J78" s="14"/>
     </row>
-    <row r="79" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I79" s="14"/>
       <c r="J79" s="14"/>
     </row>
-    <row r="80" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I80" s="14"/>
       <c r="J80" s="14"/>
     </row>
-    <row r="81" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I81" s="14"/>
       <c r="J81" s="14"/>
     </row>
-    <row r="82" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I82" s="14"/>
       <c r="J82" s="14"/>
     </row>
-    <row r="83" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I83" s="14"/>
       <c r="J83" s="14"/>
     </row>
-    <row r="84" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I84" s="14"/>
       <c r="J84" s="14"/>
     </row>
-    <row r="85" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I85" s="14"/>
       <c r="J85" s="14"/>
     </row>
-    <row r="86" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I86" s="14"/>
       <c r="J86" s="14"/>
     </row>
-    <row r="87" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I87" s="14"/>
       <c r="J87" s="14"/>
     </row>
-    <row r="88" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I88" s="14"/>
       <c r="J88" s="14"/>
     </row>
-    <row r="89" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I89" s="14"/>
       <c r="J89" s="14"/>
     </row>
-    <row r="90" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I90" s="14"/>
       <c r="J90" s="14"/>
     </row>
-    <row r="91" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I91" s="14"/>
       <c r="J91" s="14"/>
     </row>
-    <row r="92" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I92" s="14"/>
       <c r="J92" s="14"/>
     </row>
-    <row r="93" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I93" s="14"/>
       <c r="J93" s="14"/>
     </row>
-    <row r="94" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I94" s="14"/>
       <c r="J94" s="14"/>
     </row>
-    <row r="95" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I95" s="14"/>
       <c r="J95" s="14"/>
     </row>
-    <row r="96" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I96" s="14"/>
       <c r="J96" s="14"/>
     </row>
-    <row r="97" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I97" s="14"/>
       <c r="J97" s="14"/>
     </row>
-    <row r="98" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I98" s="14"/>
       <c r="J98" s="14"/>
     </row>
-    <row r="99" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I99" s="14"/>
       <c r="J99" s="14"/>
     </row>
-    <row r="100" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I100" s="14"/>
       <c r="J100" s="14"/>
     </row>
-    <row r="101" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="101" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I101" s="14"/>
       <c r="J101" s="14"/>
     </row>
-    <row r="102" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="102" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I102" s="14"/>
       <c r="J102" s="14"/>
     </row>
-    <row r="103" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="103" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I103" s="14"/>
       <c r="J103" s="14"/>
     </row>
-    <row r="104" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="104" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I104" s="14"/>
       <c r="J104" s="14"/>
     </row>
-    <row r="105" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="105" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I105" s="14"/>
       <c r="J105" s="14"/>
     </row>
-    <row r="106" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="106" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I106" s="14"/>
       <c r="J106" s="14"/>
     </row>
-    <row r="107" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="107" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I107" s="14"/>
       <c r="J107" s="14"/>
     </row>
-    <row r="108" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="108" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I108" s="14"/>
       <c r="J108" s="14"/>
     </row>
-    <row r="109" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="109" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I109" s="14"/>
       <c r="J109" s="14"/>
     </row>
-    <row r="110" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="110" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I110" s="14"/>
       <c r="J110" s="14"/>
     </row>
-    <row r="111" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="111" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I111" s="14"/>
       <c r="J111" s="14"/>
     </row>
-    <row r="112" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="112" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I112" s="14"/>
       <c r="J112" s="14"/>
     </row>
-    <row r="113" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="113" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I113" s="14"/>
       <c r="J113" s="14"/>
     </row>
-    <row r="114" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="114" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I114" s="14"/>
       <c r="J114" s="14"/>
     </row>
-    <row r="115" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="115" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I115" s="14"/>
       <c r="J115" s="14"/>
     </row>
-    <row r="116" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="116" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I116" s="14"/>
       <c r="J116" s="14"/>
     </row>
-    <row r="117" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="117" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I117" s="14"/>
       <c r="J117" s="14"/>
     </row>
-    <row r="118" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="118" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I118" s="14"/>
       <c r="J118" s="14"/>
     </row>
-    <row r="119" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="119" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I119" s="14"/>
       <c r="J119" s="14"/>
     </row>
-    <row r="120" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="120" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I120" s="14"/>
       <c r="J120" s="14"/>
     </row>
-    <row r="121" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="121" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I121" s="14"/>
       <c r="J121" s="14"/>
     </row>
-    <row r="122" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="122" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I122" s="14"/>
       <c r="J122" s="14"/>
     </row>
-    <row r="123" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="123" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I123" s="14"/>
       <c r="J123" s="14"/>
     </row>
-    <row r="124" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="124" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I124" s="14"/>
       <c r="J124" s="14"/>
     </row>
-    <row r="125" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="125" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I125" s="14"/>
       <c r="J125" s="14"/>
     </row>
-    <row r="126" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="126" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I126" s="14"/>
       <c r="J126" s="14"/>
     </row>
-    <row r="127" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="127" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I127" s="14"/>
       <c r="J127" s="14"/>
     </row>
-    <row r="128" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="128" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I128" s="14"/>
       <c r="J128" s="14"/>
     </row>
-    <row r="129" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="129" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I129" s="14"/>
       <c r="J129" s="14"/>
     </row>
-    <row r="130" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="130" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I130" s="14"/>
       <c r="J130" s="14"/>
     </row>
-    <row r="131" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="131" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I131" s="14"/>
       <c r="J131" s="14"/>
     </row>
-    <row r="132" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="132" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I132" s="14"/>
       <c r="J132" s="14"/>
     </row>
-    <row r="133" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="133" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I133" s="14"/>
       <c r="J133" s="14"/>
     </row>
-    <row r="134" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="134" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I134" s="14"/>
       <c r="J134" s="14"/>
     </row>
-    <row r="135" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="135" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I135" s="14"/>
       <c r="J135" s="14"/>
     </row>
-    <row r="136" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="136" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I136" s="14"/>
       <c r="J136" s="14"/>
     </row>
-    <row r="137" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="137" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I137" s="14"/>
       <c r="J137" s="14"/>
     </row>
-    <row r="138" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="138" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I138" s="14"/>
       <c r="J138" s="14"/>
     </row>
-    <row r="139" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="139" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I139" s="14"/>
       <c r="J139" s="14"/>
     </row>
-    <row r="140" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="140" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I140" s="14"/>
       <c r="J140" s="14"/>
     </row>
-    <row r="141" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="141" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I141" s="14"/>
       <c r="J141" s="14"/>
     </row>
-    <row r="142" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="142" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I142" s="14"/>
       <c r="J142" s="14"/>
     </row>
-    <row r="143" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="143" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I143" s="14"/>
       <c r="J143" s="14"/>
     </row>
-    <row r="144" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="144" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I144" s="14"/>
       <c r="J144" s="14"/>
     </row>
-    <row r="145" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="145" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I145" s="14"/>
       <c r="J145" s="14"/>
     </row>
-    <row r="146" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="146" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I146" s="14"/>
       <c r="J146" s="14"/>
     </row>
-    <row r="147" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="147" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I147" s="14"/>
       <c r="J147" s="14"/>
     </row>
-    <row r="148" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="148" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I148" s="14"/>
       <c r="J148" s="14"/>
     </row>
-    <row r="149" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="149" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I149" s="14"/>
       <c r="J149" s="14"/>
     </row>
-    <row r="150" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="150" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I150" s="14"/>
       <c r="J150" s="14"/>
     </row>
-    <row r="151" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="151" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I151" s="14"/>
       <c r="J151" s="14"/>
     </row>
-    <row r="152" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="152" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I152" s="14"/>
       <c r="J152" s="14"/>
     </row>
-    <row r="153" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="153" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I153" s="14"/>
       <c r="J153" s="14"/>
     </row>
-    <row r="154" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="154" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I154" s="14"/>
       <c r="J154" s="14"/>
     </row>
-    <row r="155" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="155" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I155" s="14"/>
       <c r="J155" s="14"/>
     </row>
-    <row r="156" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="156" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I156" s="14"/>
       <c r="J156" s="14"/>
     </row>
-    <row r="157" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="157" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I157" s="14"/>
       <c r="J157" s="14"/>
     </row>
-    <row r="158" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="158" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I158" s="14"/>
       <c r="J158" s="14"/>
     </row>
-    <row r="159" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="159" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I159" s="14"/>
       <c r="J159" s="14"/>
     </row>
-    <row r="160" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="160" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I160" s="14"/>
       <c r="J160" s="14"/>
     </row>
-    <row r="161" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="161" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I161" s="14"/>
       <c r="J161" s="14"/>
     </row>
-    <row r="162" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="162" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I162" s="14"/>
       <c r="J162" s="14"/>
     </row>
-    <row r="163" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="163" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I163" s="14"/>
       <c r="J163" s="14"/>
     </row>
-    <row r="164" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="164" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I164" s="14"/>
       <c r="J164" s="14"/>
     </row>
-    <row r="165" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="165" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I165" s="14"/>
       <c r="J165" s="14"/>
     </row>
-    <row r="166" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="166" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I166" s="14"/>
       <c r="J166" s="14"/>
     </row>
-    <row r="167" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="167" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I167" s="14"/>
       <c r="J167" s="14"/>
     </row>
-    <row r="168" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="168" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I168" s="14"/>
       <c r="J168" s="14"/>
     </row>
-    <row r="169" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="169" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I169" s="14"/>
       <c r="J169" s="14"/>
     </row>
-    <row r="170" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="170" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I170" s="14"/>
       <c r="J170" s="14"/>
     </row>
-    <row r="171" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="171" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I171" s="14"/>
       <c r="J171" s="14"/>
     </row>
-    <row r="172" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="172" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I172" s="14"/>
       <c r="J172" s="14"/>
     </row>
-    <row r="173" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="173" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I173" s="14"/>
       <c r="J173" s="14"/>
     </row>
-    <row r="174" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="174" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I174" s="14"/>
       <c r="J174" s="14"/>
     </row>
-    <row r="175" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="175" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I175" s="14"/>
       <c r="J175" s="14"/>
     </row>
-    <row r="176" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="176" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I176" s="14"/>
       <c r="J176" s="14"/>
     </row>
-    <row r="177" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="177" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I177" s="14"/>
       <c r="J177" s="14"/>
     </row>
-    <row r="178" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="178" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I178" s="14"/>
       <c r="J178" s="14"/>
     </row>
-    <row r="179" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="179" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I179" s="14"/>
       <c r="J179" s="14"/>
     </row>
-    <row r="180" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="180" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I180" s="14"/>
       <c r="J180" s="14"/>
     </row>
-    <row r="181" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="181" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I181" s="14"/>
       <c r="J181" s="14"/>
     </row>
-    <row r="182" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="182" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I182" s="14"/>
       <c r="J182" s="14"/>
     </row>
-    <row r="183" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="183" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I183" s="14"/>
       <c r="J183" s="14"/>
     </row>
-    <row r="184" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="184" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I184" s="14"/>
       <c r="J184" s="14"/>
     </row>
-    <row r="185" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="185" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I185" s="14"/>
       <c r="J185" s="14"/>
     </row>
-    <row r="186" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="186" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I186" s="14"/>
       <c r="J186" s="14"/>
     </row>
-    <row r="187" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="187" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I187" s="14"/>
       <c r="J187" s="14"/>
     </row>
-    <row r="188" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="188" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I188" s="14"/>
       <c r="J188" s="14"/>
     </row>
-    <row r="189" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="189" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I189" s="14"/>
       <c r="J189" s="14"/>
     </row>
-    <row r="190" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="190" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I190" s="14"/>
       <c r="J190" s="14"/>
     </row>
-    <row r="191" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="191" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I191" s="14"/>
       <c r="J191" s="14"/>
     </row>
-    <row r="192" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="192" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I192" s="14"/>
       <c r="J192" s="14"/>
     </row>
-    <row r="193" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="193" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I193" s="14"/>
       <c r="J193" s="14"/>
     </row>
-    <row r="194" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="194" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I194" s="14"/>
       <c r="J194" s="14"/>
     </row>
-    <row r="195" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="195" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I195" s="14"/>
       <c r="J195" s="14"/>
     </row>
-    <row r="196" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="196" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I196" s="14"/>
       <c r="J196" s="14"/>
     </row>
-    <row r="197" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="197" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I197" s="14"/>
       <c r="J197" s="14"/>
     </row>
-    <row r="198" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="198" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I198" s="14"/>
       <c r="J198" s="14"/>
     </row>
-    <row r="199" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="199" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I199" s="14"/>
       <c r="J199" s="14"/>
     </row>
-    <row r="200" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="200" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I200" s="14"/>
       <c r="J200" s="14"/>
     </row>
-    <row r="201" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="201" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I201" s="14"/>
       <c r="J201" s="14"/>
     </row>
-    <row r="202" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="202" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I202" s="14"/>
       <c r="J202" s="14"/>
     </row>
-    <row r="203" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="203" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I203" s="14"/>
       <c r="J203" s="14"/>
     </row>
-    <row r="204" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="204" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I204" s="14"/>
       <c r="J204" s="14"/>
     </row>
-    <row r="205" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="205" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I205" s="14"/>
       <c r="J205" s="14"/>
     </row>
-    <row r="206" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="206" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I206" s="14"/>
       <c r="J206" s="14"/>
     </row>
-    <row r="207" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="207" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I207" s="14"/>
       <c r="J207" s="14"/>
     </row>
-    <row r="208" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="208" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I208" s="14"/>
       <c r="J208" s="14"/>
     </row>
-    <row r="209" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="209" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I209" s="14"/>
       <c r="J209" s="14"/>
     </row>
-    <row r="210" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="210" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I210" s="14"/>
       <c r="J210" s="14"/>
     </row>
-    <row r="211" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="211" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I211" s="14"/>
       <c r="J211" s="14"/>
     </row>
-    <row r="212" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="212" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I212" s="14"/>
       <c r="J212" s="14"/>
     </row>
-    <row r="213" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="213" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I213" s="14"/>
       <c r="J213" s="14"/>
     </row>
-    <row r="214" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="214" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I214" s="14"/>
       <c r="J214" s="14"/>
     </row>
-    <row r="215" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="215" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I215" s="14"/>
       <c r="J215" s="14"/>
     </row>
-    <row r="216" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="216" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I216" s="14"/>
       <c r="J216" s="14"/>
     </row>
-    <row r="217" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="217" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I217" s="14"/>
       <c r="J217" s="14"/>
     </row>
-    <row r="218" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="218" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I218" s="14"/>
       <c r="J218" s="14"/>
     </row>
-    <row r="219" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="219" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I219" s="14"/>
       <c r="J219" s="14"/>
     </row>
-    <row r="220" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="220" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I220" s="14"/>
       <c r="J220" s="14"/>
     </row>
-    <row r="221" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="221" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I221" s="14"/>
       <c r="J221" s="14"/>
     </row>
-    <row r="222" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="222" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I222" s="14"/>
       <c r="J222" s="14"/>
     </row>
-    <row r="223" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="223" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I223" s="14"/>
       <c r="J223" s="14"/>
     </row>
-    <row r="224" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="224" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I224" s="14"/>
       <c r="J224" s="14"/>
     </row>
-    <row r="225" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="225" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I225" s="14"/>
       <c r="J225" s="14"/>
     </row>
-    <row r="226" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="226" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I226" s="14"/>
       <c r="J226" s="14"/>
     </row>
-    <row r="227" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="227" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I227" s="14"/>
       <c r="J227" s="14"/>
     </row>
-    <row r="228" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="228" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I228" s="14"/>
       <c r="J228" s="14"/>
     </row>
-    <row r="229" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="229" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I229" s="14"/>
       <c r="J229" s="14"/>
     </row>
-    <row r="230" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="230" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I230" s="14"/>
       <c r="J230" s="14"/>
     </row>
-    <row r="231" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="231" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I231" s="14"/>
       <c r="J231" s="14"/>
     </row>
-    <row r="232" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="232" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I232" s="14"/>
       <c r="J232" s="14"/>
     </row>
-    <row r="233" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="233" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I233" s="14"/>
       <c r="J233" s="14"/>
     </row>
-    <row r="234" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="234" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I234" s="14"/>
       <c r="J234" s="14"/>
     </row>
-    <row r="235" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="235" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I235" s="14"/>
       <c r="J235" s="14"/>
     </row>
-    <row r="236" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="236" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I236" s="14"/>
       <c r="J236" s="14"/>
     </row>
-    <row r="237" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="237" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I237" s="14"/>
       <c r="J237" s="14"/>
     </row>
-    <row r="238" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="238" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I238" s="14"/>
       <c r="J238" s="14"/>
     </row>
-    <row r="239" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="239" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I239" s="14"/>
       <c r="J239" s="14"/>
     </row>
-    <row r="240" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="240" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I240" s="14"/>
       <c r="J240" s="14"/>
     </row>
-    <row r="241" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="241" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I241" s="14"/>
       <c r="J241" s="14"/>
     </row>
-    <row r="242" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="242" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I242" s="14"/>
       <c r="J242" s="14"/>
     </row>
-    <row r="243" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="243" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I243" s="14"/>
       <c r="J243" s="14"/>
     </row>
-    <row r="244" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="244" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I244" s="14"/>
       <c r="J244" s="14"/>
     </row>
-    <row r="245" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="245" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I245" s="14"/>
       <c r="J245" s="14"/>
     </row>
-    <row r="246" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="246" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I246" s="14"/>
       <c r="J246" s="14"/>
     </row>
-    <row r="247" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="247" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I247" s="14"/>
       <c r="J247" s="14"/>
     </row>
-    <row r="248" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="248" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I248" s="14"/>
       <c r="J248" s="14"/>
     </row>
-    <row r="249" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="249" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I249" s="14"/>
       <c r="J249" s="14"/>
     </row>
-    <row r="250" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="250" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I250" s="14"/>
       <c r="J250" s="14"/>
     </row>
-    <row r="251" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="251" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I251" s="14"/>
       <c r="J251" s="14"/>
     </row>
-    <row r="252" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="252" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I252" s="14"/>
       <c r="J252" s="14"/>
     </row>
-    <row r="253" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="253" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I253" s="14"/>
       <c r="J253" s="14"/>
     </row>
-    <row r="254" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="254" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I254" s="14"/>
       <c r="J254" s="14"/>
     </row>
-    <row r="255" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="255" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I255" s="14"/>
       <c r="J255" s="14"/>
     </row>
-    <row r="256" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="256" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I256" s="14"/>
       <c r="J256" s="14"/>
     </row>
-    <row r="257" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="257" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I257" s="14"/>
       <c r="J257" s="14"/>
     </row>
-    <row r="258" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="258" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I258" s="14"/>
       <c r="J258" s="14"/>
     </row>
-    <row r="259" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="259" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I259" s="14"/>
       <c r="J259" s="14"/>
     </row>
-    <row r="260" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="260" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I260" s="14"/>
       <c r="J260" s="14"/>
     </row>
-    <row r="261" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="261" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I261" s="14"/>
       <c r="J261" s="14"/>
     </row>
-    <row r="262" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="262" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I262" s="14"/>
       <c r="J262" s="14"/>
     </row>
-    <row r="263" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="263" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I263" s="14"/>
       <c r="J263" s="14"/>
     </row>
-    <row r="264" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="264" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I264" s="14"/>
       <c r="J264" s="14"/>
     </row>
-    <row r="265" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="265" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I265" s="14"/>
       <c r="J265" s="14"/>
     </row>
-    <row r="266" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="266" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I266" s="14"/>
       <c r="J266" s="14"/>
     </row>
-    <row r="267" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="267" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I267" s="14"/>
       <c r="J267" s="14"/>
     </row>
-    <row r="268" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="268" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I268" s="14"/>
       <c r="J268" s="14"/>
     </row>
-    <row r="269" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="269" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I269" s="14"/>
       <c r="J269" s="14"/>
     </row>
-    <row r="270" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="270" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I270" s="14"/>
       <c r="J270" s="14"/>
     </row>
-    <row r="271" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="271" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I271" s="14"/>
       <c r="J271" s="14"/>
     </row>
-    <row r="272" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="272" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I272" s="14"/>
       <c r="J272" s="14"/>
     </row>
-    <row r="273" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="273" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I273" s="14"/>
       <c r="J273" s="14"/>
     </row>
-    <row r="274" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="274" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I274" s="14"/>
       <c r="J274" s="14"/>
     </row>
-    <row r="275" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="275" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I275" s="14"/>
       <c r="J275" s="14"/>
     </row>
-    <row r="276" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="276" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I276" s="14"/>
       <c r="J276" s="14"/>
     </row>
-    <row r="277" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="277" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I277" s="14"/>
       <c r="J277" s="14"/>
     </row>
-    <row r="278" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="278" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I278" s="14"/>
       <c r="J278" s="14"/>
     </row>
-    <row r="279" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="279" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I279" s="14"/>
       <c r="J279" s="14"/>
     </row>
-    <row r="280" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="280" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I280" s="14"/>
       <c r="J280" s="14"/>
     </row>
-    <row r="281" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="281" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I281" s="14"/>
       <c r="J281" s="14"/>
     </row>
-    <row r="282" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="282" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I282" s="14"/>
       <c r="J282" s="14"/>
     </row>
-    <row r="283" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="283" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I283" s="14"/>
       <c r="J283" s="14"/>
     </row>
-    <row r="284" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="284" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I284" s="14"/>
       <c r="J284" s="14"/>
     </row>
-    <row r="285" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="285" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I285" s="14"/>
       <c r="J285" s="14"/>
     </row>
-    <row r="286" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="286" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I286" s="14"/>
       <c r="J286" s="14"/>
     </row>
-    <row r="287" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="287" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I287" s="14"/>
       <c r="J287" s="14"/>
     </row>
-    <row r="288" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="288" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I288" s="14"/>
       <c r="J288" s="14"/>
     </row>
-    <row r="289" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="289" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I289" s="14"/>
       <c r="J289" s="14"/>
     </row>
-    <row r="290" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="290" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I290" s="14"/>
       <c r="J290" s="14"/>
     </row>
-    <row r="291" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="291" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I291" s="14"/>
       <c r="J291" s="14"/>
     </row>
-    <row r="292" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="292" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I292" s="14"/>
       <c r="J292" s="14"/>
     </row>
-    <row r="293" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="293" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I293" s="14"/>
       <c r="J293" s="14"/>
     </row>
-    <row r="294" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="294" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I294" s="14"/>
       <c r="J294" s="14"/>
     </row>
-    <row r="295" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="295" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I295" s="14"/>
       <c r="J295" s="14"/>
     </row>
-    <row r="296" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="296" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I296" s="14"/>
       <c r="J296" s="14"/>
     </row>
-    <row r="297" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="297" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I297" s="14"/>
       <c r="J297" s="14"/>
     </row>
-    <row r="298" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="298" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I298" s="14"/>
       <c r="J298" s="14"/>
     </row>
-    <row r="299" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="299" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I299" s="14"/>
       <c r="J299" s="14"/>
     </row>
-    <row r="300" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="300" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I300" s="14"/>
       <c r="J300" s="14"/>
     </row>
-    <row r="301" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="301" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I301" s="14"/>
       <c r="J301" s="14"/>
     </row>
-    <row r="302" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="302" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I302" s="14"/>
       <c r="J302" s="14"/>
     </row>
-    <row r="303" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="303" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I303" s="14"/>
       <c r="J303" s="14"/>
     </row>
-    <row r="304" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="304" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I304" s="14"/>
       <c r="J304" s="14"/>
     </row>
-    <row r="305" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="305" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I305" s="14"/>
       <c r="J305" s="14"/>
     </row>
-    <row r="306" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="306" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I306" s="14"/>
       <c r="J306" s="14"/>
     </row>
-    <row r="307" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="307" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I307" s="14"/>
       <c r="J307" s="14"/>
     </row>
-    <row r="308" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="308" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I308" s="14"/>
       <c r="J308" s="14"/>
     </row>
-    <row r="309" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="309" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I309" s="14"/>
       <c r="J309" s="14"/>
     </row>
-    <row r="310" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="310" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I310" s="14"/>
       <c r="J310" s="14"/>
     </row>
-    <row r="311" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="311" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I311" s="14"/>
       <c r="J311" s="14"/>
     </row>
-    <row r="312" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="312" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I312" s="14"/>
       <c r="J312" s="14"/>
     </row>
-    <row r="313" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="313" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I313" s="14"/>
       <c r="J313" s="14"/>
     </row>
-    <row r="314" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="314" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I314" s="14"/>
       <c r="J314" s="14"/>
     </row>
-    <row r="315" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="315" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I315" s="14"/>
       <c r="J315" s="14"/>
     </row>
-    <row r="316" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="316" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I316" s="14"/>
       <c r="J316" s="14"/>
     </row>
-    <row r="317" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="317" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I317" s="14"/>
       <c r="J317" s="14"/>
     </row>
-    <row r="318" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="318" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I318" s="14"/>
       <c r="J318" s="14"/>
     </row>
-    <row r="319" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="319" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I319" s="14"/>
       <c r="J319" s="14"/>
     </row>
-    <row r="320" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="320" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I320" s="14"/>
       <c r="J320" s="14"/>
     </row>
-    <row r="321" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="321" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I321" s="14"/>
       <c r="J321" s="14"/>
     </row>
-    <row r="322" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="322" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I322" s="14"/>
       <c r="J322" s="14"/>
     </row>
-    <row r="323" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="323" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I323" s="14"/>
       <c r="J323" s="14"/>
     </row>
-    <row r="324" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="324" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I324" s="14"/>
       <c r="J324" s="14"/>
     </row>
-    <row r="325" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="325" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I325" s="14"/>
       <c r="J325" s="14"/>
     </row>
-    <row r="326" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="326" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I326" s="14"/>
       <c r="J326" s="14"/>
     </row>
-    <row r="327" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="327" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I327" s="14"/>
       <c r="J327" s="14"/>
     </row>
-    <row r="328" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="328" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I328" s="14"/>
       <c r="J328" s="14"/>
     </row>
-    <row r="329" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="329" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I329" s="14"/>
       <c r="J329" s="14"/>
     </row>
-    <row r="330" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="330" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I330" s="14"/>
       <c r="J330" s="14"/>
     </row>
-    <row r="331" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="331" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I331" s="14"/>
       <c r="J331" s="14"/>
     </row>
-    <row r="332" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="332" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I332" s="14"/>
       <c r="J332" s="14"/>
     </row>
-    <row r="333" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="333" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I333" s="14"/>
       <c r="J333" s="14"/>
     </row>
-    <row r="334" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="334" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I334" s="14"/>
       <c r="J334" s="14"/>
     </row>
-    <row r="335" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="335" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I335" s="14"/>
       <c r="J335" s="14"/>
     </row>
-    <row r="336" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="336" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I336" s="14"/>
       <c r="J336" s="14"/>
     </row>
-    <row r="337" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="337" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I337" s="14"/>
       <c r="J337" s="14"/>
     </row>
-    <row r="338" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="338" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I338" s="14"/>
       <c r="J338" s="14"/>
     </row>
-    <row r="339" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="339" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I339" s="14"/>
       <c r="J339" s="14"/>
     </row>
-    <row r="340" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="340" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I340" s="14"/>
       <c r="J340" s="14"/>
     </row>
-    <row r="341" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="341" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I341" s="14"/>
       <c r="J341" s="14"/>
     </row>
-    <row r="342" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="342" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I342" s="14"/>
       <c r="J342" s="14"/>
     </row>
-    <row r="343" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="343" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I343" s="14"/>
       <c r="J343" s="14"/>
     </row>
-    <row r="344" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="344" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I344" s="14"/>
       <c r="J344" s="14"/>
     </row>
-    <row r="345" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="345" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I345" s="14"/>
       <c r="J345" s="14"/>
     </row>
-    <row r="346" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="346" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I346" s="14"/>
       <c r="J346" s="14"/>
     </row>
-    <row r="347" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="347" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I347" s="14"/>
       <c r="J347" s="14"/>
     </row>
-    <row r="348" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="348" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I348" s="14"/>
       <c r="J348" s="14"/>
     </row>
-    <row r="349" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="349" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I349" s="14"/>
       <c r="J349" s="14"/>
     </row>
-    <row r="350" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="350" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I350" s="14"/>
       <c r="J350" s="14"/>
     </row>
-    <row r="351" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="351" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I351" s="14"/>
       <c r="J351" s="14"/>
     </row>
-    <row r="352" spans="9:10" x14ac:dyDescent="0.3">
+    <row r="352" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I352" s="14"/>
       <c r="J352" s="14"/>
     </row>
@@ -2832,6 +2822,1859 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E10B533E-38A2-4A18-91F9-81A95CC6AC6B}">
+  <sheetPr>
+    <tabColor theme="0" tint="-0.14999847407452621"/>
+  </sheetPr>
+  <dimension ref="A1:AF352"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="5" width="6.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" style="1" customWidth="1"/>
+    <col min="9" max="10" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="50" width="6.7109375" style="1" customWidth="1"/>
+    <col min="51" max="16384" width="8.7109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="N1" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="8"/>
+      <c r="AE1" s="8"/>
+      <c r="AF1" s="2"/>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A2" s="7">
+        <v>2E-3</v>
+      </c>
+      <c r="B2" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="C2" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D2" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="E2" s="7">
+        <v>0</v>
+      </c>
+      <c r="F2" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="G2" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="H2" s="7">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="I2" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="J2" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="K2" s="7">
+        <f>1/10</f>
+        <v>0.1</v>
+      </c>
+      <c r="L2" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="M2" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="N2" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="7"/>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="7"/>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="7"/>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="7"/>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="7"/>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="7"/>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="7"/>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="7"/>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="7"/>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="7"/>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="7"/>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="7"/>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="7"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="7"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="7"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="7"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="7"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="7"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="7"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="7"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="7"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="7"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="7"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="7"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="7"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+    </row>
+    <row r="33" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
+    </row>
+    <row r="34" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I34" s="14"/>
+      <c r="J34" s="14"/>
+    </row>
+    <row r="35" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+    </row>
+    <row r="36" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+    </row>
+    <row r="37" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+    </row>
+    <row r="38" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+    </row>
+    <row r="39" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I39" s="14"/>
+      <c r="J39" s="14"/>
+    </row>
+    <row r="40" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+    </row>
+    <row r="41" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
+    </row>
+    <row r="42" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+    </row>
+    <row r="43" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I43" s="14"/>
+      <c r="J43" s="14"/>
+    </row>
+    <row r="44" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I44" s="14"/>
+      <c r="J44" s="14"/>
+    </row>
+    <row r="45" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I45" s="14"/>
+      <c r="J45" s="14"/>
+    </row>
+    <row r="46" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I46" s="14"/>
+      <c r="J46" s="14"/>
+    </row>
+    <row r="47" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I47" s="14"/>
+      <c r="J47" s="14"/>
+    </row>
+    <row r="48" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I48" s="14"/>
+      <c r="J48" s="14"/>
+    </row>
+    <row r="49" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I49" s="14"/>
+      <c r="J49" s="14"/>
+    </row>
+    <row r="50" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I50" s="14"/>
+      <c r="J50" s="14"/>
+    </row>
+    <row r="51" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
+    </row>
+    <row r="52" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I52" s="14"/>
+      <c r="J52" s="14"/>
+    </row>
+    <row r="53" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I53" s="14"/>
+      <c r="J53" s="14"/>
+    </row>
+    <row r="54" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I54" s="14"/>
+      <c r="J54" s="14"/>
+    </row>
+    <row r="55" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I55" s="14"/>
+      <c r="J55" s="14"/>
+    </row>
+    <row r="56" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I56" s="14"/>
+      <c r="J56" s="14"/>
+    </row>
+    <row r="57" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I57" s="14"/>
+      <c r="J57" s="14"/>
+    </row>
+    <row r="58" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I58" s="14"/>
+      <c r="J58" s="14"/>
+    </row>
+    <row r="59" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I59" s="14"/>
+      <c r="J59" s="14"/>
+    </row>
+    <row r="60" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I60" s="14"/>
+      <c r="J60" s="14"/>
+    </row>
+    <row r="61" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I61" s="14"/>
+      <c r="J61" s="14"/>
+    </row>
+    <row r="62" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I62" s="14"/>
+      <c r="J62" s="14"/>
+    </row>
+    <row r="63" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I63" s="14"/>
+      <c r="J63" s="14"/>
+    </row>
+    <row r="64" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I64" s="14"/>
+      <c r="J64" s="14"/>
+    </row>
+    <row r="65" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I65" s="14"/>
+      <c r="J65" s="14"/>
+    </row>
+    <row r="66" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I66" s="14"/>
+      <c r="J66" s="14"/>
+    </row>
+    <row r="67" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I67" s="14"/>
+      <c r="J67" s="14"/>
+    </row>
+    <row r="68" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I68" s="14"/>
+      <c r="J68" s="14"/>
+    </row>
+    <row r="69" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I69" s="14"/>
+      <c r="J69" s="14"/>
+    </row>
+    <row r="70" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I70" s="14"/>
+      <c r="J70" s="14"/>
+    </row>
+    <row r="71" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I71" s="14"/>
+      <c r="J71" s="14"/>
+    </row>
+    <row r="72" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I72" s="14"/>
+      <c r="J72" s="14"/>
+    </row>
+    <row r="73" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I73" s="14"/>
+      <c r="J73" s="14"/>
+    </row>
+    <row r="74" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I74" s="14"/>
+      <c r="J74" s="14"/>
+    </row>
+    <row r="75" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I75" s="14"/>
+      <c r="J75" s="14"/>
+    </row>
+    <row r="76" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I76" s="14"/>
+      <c r="J76" s="14"/>
+    </row>
+    <row r="77" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I77" s="14"/>
+      <c r="J77" s="14"/>
+    </row>
+    <row r="78" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I78" s="14"/>
+      <c r="J78" s="14"/>
+    </row>
+    <row r="79" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I79" s="14"/>
+      <c r="J79" s="14"/>
+    </row>
+    <row r="80" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I80" s="14"/>
+      <c r="J80" s="14"/>
+    </row>
+    <row r="81" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I81" s="14"/>
+      <c r="J81" s="14"/>
+    </row>
+    <row r="82" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I82" s="14"/>
+      <c r="J82" s="14"/>
+    </row>
+    <row r="83" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I83" s="14"/>
+      <c r="J83" s="14"/>
+    </row>
+    <row r="84" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I84" s="14"/>
+      <c r="J84" s="14"/>
+    </row>
+    <row r="85" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I85" s="14"/>
+      <c r="J85" s="14"/>
+    </row>
+    <row r="86" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I86" s="14"/>
+      <c r="J86" s="14"/>
+    </row>
+    <row r="87" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I87" s="14"/>
+      <c r="J87" s="14"/>
+    </row>
+    <row r="88" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I88" s="14"/>
+      <c r="J88" s="14"/>
+    </row>
+    <row r="89" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I89" s="14"/>
+      <c r="J89" s="14"/>
+    </row>
+    <row r="90" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I90" s="14"/>
+      <c r="J90" s="14"/>
+    </row>
+    <row r="91" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I91" s="14"/>
+      <c r="J91" s="14"/>
+    </row>
+    <row r="92" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I92" s="14"/>
+      <c r="J92" s="14"/>
+    </row>
+    <row r="93" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I93" s="14"/>
+      <c r="J93" s="14"/>
+    </row>
+    <row r="94" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I94" s="14"/>
+      <c r="J94" s="14"/>
+    </row>
+    <row r="95" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I95" s="14"/>
+      <c r="J95" s="14"/>
+    </row>
+    <row r="96" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I96" s="14"/>
+      <c r="J96" s="14"/>
+    </row>
+    <row r="97" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I97" s="14"/>
+      <c r="J97" s="14"/>
+    </row>
+    <row r="98" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I98" s="14"/>
+      <c r="J98" s="14"/>
+    </row>
+    <row r="99" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I99" s="14"/>
+      <c r="J99" s="14"/>
+    </row>
+    <row r="100" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I100" s="14"/>
+      <c r="J100" s="14"/>
+    </row>
+    <row r="101" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I101" s="14"/>
+      <c r="J101" s="14"/>
+    </row>
+    <row r="102" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I102" s="14"/>
+      <c r="J102" s="14"/>
+    </row>
+    <row r="103" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I103" s="14"/>
+      <c r="J103" s="14"/>
+    </row>
+    <row r="104" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I104" s="14"/>
+      <c r="J104" s="14"/>
+    </row>
+    <row r="105" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I105" s="14"/>
+      <c r="J105" s="14"/>
+    </row>
+    <row r="106" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I106" s="14"/>
+      <c r="J106" s="14"/>
+    </row>
+    <row r="107" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I107" s="14"/>
+      <c r="J107" s="14"/>
+    </row>
+    <row r="108" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I108" s="14"/>
+      <c r="J108" s="14"/>
+    </row>
+    <row r="109" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I109" s="14"/>
+      <c r="J109" s="14"/>
+    </row>
+    <row r="110" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I110" s="14"/>
+      <c r="J110" s="14"/>
+    </row>
+    <row r="111" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I111" s="14"/>
+      <c r="J111" s="14"/>
+    </row>
+    <row r="112" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I112" s="14"/>
+      <c r="J112" s="14"/>
+    </row>
+    <row r="113" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I113" s="14"/>
+      <c r="J113" s="14"/>
+    </row>
+    <row r="114" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I114" s="14"/>
+      <c r="J114" s="14"/>
+    </row>
+    <row r="115" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I115" s="14"/>
+      <c r="J115" s="14"/>
+    </row>
+    <row r="116" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I116" s="14"/>
+      <c r="J116" s="14"/>
+    </row>
+    <row r="117" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I117" s="14"/>
+      <c r="J117" s="14"/>
+    </row>
+    <row r="118" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I118" s="14"/>
+      <c r="J118" s="14"/>
+    </row>
+    <row r="119" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I119" s="14"/>
+      <c r="J119" s="14"/>
+    </row>
+    <row r="120" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I120" s="14"/>
+      <c r="J120" s="14"/>
+    </row>
+    <row r="121" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I121" s="14"/>
+      <c r="J121" s="14"/>
+    </row>
+    <row r="122" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I122" s="14"/>
+      <c r="J122" s="14"/>
+    </row>
+    <row r="123" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I123" s="14"/>
+      <c r="J123" s="14"/>
+    </row>
+    <row r="124" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I124" s="14"/>
+      <c r="J124" s="14"/>
+    </row>
+    <row r="125" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I125" s="14"/>
+      <c r="J125" s="14"/>
+    </row>
+    <row r="126" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I126" s="14"/>
+      <c r="J126" s="14"/>
+    </row>
+    <row r="127" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I127" s="14"/>
+      <c r="J127" s="14"/>
+    </row>
+    <row r="128" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I128" s="14"/>
+      <c r="J128" s="14"/>
+    </row>
+    <row r="129" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I129" s="14"/>
+      <c r="J129" s="14"/>
+    </row>
+    <row r="130" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I130" s="14"/>
+      <c r="J130" s="14"/>
+    </row>
+    <row r="131" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I131" s="14"/>
+      <c r="J131" s="14"/>
+    </row>
+    <row r="132" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I132" s="14"/>
+      <c r="J132" s="14"/>
+    </row>
+    <row r="133" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I133" s="14"/>
+      <c r="J133" s="14"/>
+    </row>
+    <row r="134" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I134" s="14"/>
+      <c r="J134" s="14"/>
+    </row>
+    <row r="135" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I135" s="14"/>
+      <c r="J135" s="14"/>
+    </row>
+    <row r="136" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I136" s="14"/>
+      <c r="J136" s="14"/>
+    </row>
+    <row r="137" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I137" s="14"/>
+      <c r="J137" s="14"/>
+    </row>
+    <row r="138" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I138" s="14"/>
+      <c r="J138" s="14"/>
+    </row>
+    <row r="139" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I139" s="14"/>
+      <c r="J139" s="14"/>
+    </row>
+    <row r="140" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I140" s="14"/>
+      <c r="J140" s="14"/>
+    </row>
+    <row r="141" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I141" s="14"/>
+      <c r="J141" s="14"/>
+    </row>
+    <row r="142" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I142" s="14"/>
+      <c r="J142" s="14"/>
+    </row>
+    <row r="143" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I143" s="14"/>
+      <c r="J143" s="14"/>
+    </row>
+    <row r="144" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I144" s="14"/>
+      <c r="J144" s="14"/>
+    </row>
+    <row r="145" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I145" s="14"/>
+      <c r="J145" s="14"/>
+    </row>
+    <row r="146" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I146" s="14"/>
+      <c r="J146" s="14"/>
+    </row>
+    <row r="147" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I147" s="14"/>
+      <c r="J147" s="14"/>
+    </row>
+    <row r="148" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I148" s="14"/>
+      <c r="J148" s="14"/>
+    </row>
+    <row r="149" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I149" s="14"/>
+      <c r="J149" s="14"/>
+    </row>
+    <row r="150" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I150" s="14"/>
+      <c r="J150" s="14"/>
+    </row>
+    <row r="151" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I151" s="14"/>
+      <c r="J151" s="14"/>
+    </row>
+    <row r="152" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I152" s="14"/>
+      <c r="J152" s="14"/>
+    </row>
+    <row r="153" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I153" s="14"/>
+      <c r="J153" s="14"/>
+    </row>
+    <row r="154" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I154" s="14"/>
+      <c r="J154" s="14"/>
+    </row>
+    <row r="155" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I155" s="14"/>
+      <c r="J155" s="14"/>
+    </row>
+    <row r="156" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I156" s="14"/>
+      <c r="J156" s="14"/>
+    </row>
+    <row r="157" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I157" s="14"/>
+      <c r="J157" s="14"/>
+    </row>
+    <row r="158" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I158" s="14"/>
+      <c r="J158" s="14"/>
+    </row>
+    <row r="159" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I159" s="14"/>
+      <c r="J159" s="14"/>
+    </row>
+    <row r="160" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I160" s="14"/>
+      <c r="J160" s="14"/>
+    </row>
+    <row r="161" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I161" s="14"/>
+      <c r="J161" s="14"/>
+    </row>
+    <row r="162" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I162" s="14"/>
+      <c r="J162" s="14"/>
+    </row>
+    <row r="163" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I163" s="14"/>
+      <c r="J163" s="14"/>
+    </row>
+    <row r="164" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I164" s="14"/>
+      <c r="J164" s="14"/>
+    </row>
+    <row r="165" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I165" s="14"/>
+      <c r="J165" s="14"/>
+    </row>
+    <row r="166" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I166" s="14"/>
+      <c r="J166" s="14"/>
+    </row>
+    <row r="167" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I167" s="14"/>
+      <c r="J167" s="14"/>
+    </row>
+    <row r="168" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I168" s="14"/>
+      <c r="J168" s="14"/>
+    </row>
+    <row r="169" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I169" s="14"/>
+      <c r="J169" s="14"/>
+    </row>
+    <row r="170" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I170" s="14"/>
+      <c r="J170" s="14"/>
+    </row>
+    <row r="171" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I171" s="14"/>
+      <c r="J171" s="14"/>
+    </row>
+    <row r="172" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I172" s="14"/>
+      <c r="J172" s="14"/>
+    </row>
+    <row r="173" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I173" s="14"/>
+      <c r="J173" s="14"/>
+    </row>
+    <row r="174" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I174" s="14"/>
+      <c r="J174" s="14"/>
+    </row>
+    <row r="175" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I175" s="14"/>
+      <c r="J175" s="14"/>
+    </row>
+    <row r="176" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I176" s="14"/>
+      <c r="J176" s="14"/>
+    </row>
+    <row r="177" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I177" s="14"/>
+      <c r="J177" s="14"/>
+    </row>
+    <row r="178" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I178" s="14"/>
+      <c r="J178" s="14"/>
+    </row>
+    <row r="179" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I179" s="14"/>
+      <c r="J179" s="14"/>
+    </row>
+    <row r="180" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I180" s="14"/>
+      <c r="J180" s="14"/>
+    </row>
+    <row r="181" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I181" s="14"/>
+      <c r="J181" s="14"/>
+    </row>
+    <row r="182" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I182" s="14"/>
+      <c r="J182" s="14"/>
+    </row>
+    <row r="183" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I183" s="14"/>
+      <c r="J183" s="14"/>
+    </row>
+    <row r="184" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I184" s="14"/>
+      <c r="J184" s="14"/>
+    </row>
+    <row r="185" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I185" s="14"/>
+      <c r="J185" s="14"/>
+    </row>
+    <row r="186" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I186" s="14"/>
+      <c r="J186" s="14"/>
+    </row>
+    <row r="187" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I187" s="14"/>
+      <c r="J187" s="14"/>
+    </row>
+    <row r="188" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I188" s="14"/>
+      <c r="J188" s="14"/>
+    </row>
+    <row r="189" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I189" s="14"/>
+      <c r="J189" s="14"/>
+    </row>
+    <row r="190" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I190" s="14"/>
+      <c r="J190" s="14"/>
+    </row>
+    <row r="191" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I191" s="14"/>
+      <c r="J191" s="14"/>
+    </row>
+    <row r="192" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I192" s="14"/>
+      <c r="J192" s="14"/>
+    </row>
+    <row r="193" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I193" s="14"/>
+      <c r="J193" s="14"/>
+    </row>
+    <row r="194" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I194" s="14"/>
+      <c r="J194" s="14"/>
+    </row>
+    <row r="195" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I195" s="14"/>
+      <c r="J195" s="14"/>
+    </row>
+    <row r="196" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I196" s="14"/>
+      <c r="J196" s="14"/>
+    </row>
+    <row r="197" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I197" s="14"/>
+      <c r="J197" s="14"/>
+    </row>
+    <row r="198" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I198" s="14"/>
+      <c r="J198" s="14"/>
+    </row>
+    <row r="199" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I199" s="14"/>
+      <c r="J199" s="14"/>
+    </row>
+    <row r="200" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I200" s="14"/>
+      <c r="J200" s="14"/>
+    </row>
+    <row r="201" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I201" s="14"/>
+      <c r="J201" s="14"/>
+    </row>
+    <row r="202" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I202" s="14"/>
+      <c r="J202" s="14"/>
+    </row>
+    <row r="203" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I203" s="14"/>
+      <c r="J203" s="14"/>
+    </row>
+    <row r="204" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I204" s="14"/>
+      <c r="J204" s="14"/>
+    </row>
+    <row r="205" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I205" s="14"/>
+      <c r="J205" s="14"/>
+    </row>
+    <row r="206" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I206" s="14"/>
+      <c r="J206" s="14"/>
+    </row>
+    <row r="207" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I207" s="14"/>
+      <c r="J207" s="14"/>
+    </row>
+    <row r="208" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I208" s="14"/>
+      <c r="J208" s="14"/>
+    </row>
+    <row r="209" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I209" s="14"/>
+      <c r="J209" s="14"/>
+    </row>
+    <row r="210" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I210" s="14"/>
+      <c r="J210" s="14"/>
+    </row>
+    <row r="211" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I211" s="14"/>
+      <c r="J211" s="14"/>
+    </row>
+    <row r="212" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I212" s="14"/>
+      <c r="J212" s="14"/>
+    </row>
+    <row r="213" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I213" s="14"/>
+      <c r="J213" s="14"/>
+    </row>
+    <row r="214" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I214" s="14"/>
+      <c r="J214" s="14"/>
+    </row>
+    <row r="215" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I215" s="14"/>
+      <c r="J215" s="14"/>
+    </row>
+    <row r="216" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I216" s="14"/>
+      <c r="J216" s="14"/>
+    </row>
+    <row r="217" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I217" s="14"/>
+      <c r="J217" s="14"/>
+    </row>
+    <row r="218" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I218" s="14"/>
+      <c r="J218" s="14"/>
+    </row>
+    <row r="219" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I219" s="14"/>
+      <c r="J219" s="14"/>
+    </row>
+    <row r="220" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I220" s="14"/>
+      <c r="J220" s="14"/>
+    </row>
+    <row r="221" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I221" s="14"/>
+      <c r="J221" s="14"/>
+    </row>
+    <row r="222" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I222" s="14"/>
+      <c r="J222" s="14"/>
+    </row>
+    <row r="223" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I223" s="14"/>
+      <c r="J223" s="14"/>
+    </row>
+    <row r="224" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I224" s="14"/>
+      <c r="J224" s="14"/>
+    </row>
+    <row r="225" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I225" s="14"/>
+      <c r="J225" s="14"/>
+    </row>
+    <row r="226" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I226" s="14"/>
+      <c r="J226" s="14"/>
+    </row>
+    <row r="227" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I227" s="14"/>
+      <c r="J227" s="14"/>
+    </row>
+    <row r="228" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I228" s="14"/>
+      <c r="J228" s="14"/>
+    </row>
+    <row r="229" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I229" s="14"/>
+      <c r="J229" s="14"/>
+    </row>
+    <row r="230" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I230" s="14"/>
+      <c r="J230" s="14"/>
+    </row>
+    <row r="231" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I231" s="14"/>
+      <c r="J231" s="14"/>
+    </row>
+    <row r="232" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I232" s="14"/>
+      <c r="J232" s="14"/>
+    </row>
+    <row r="233" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I233" s="14"/>
+      <c r="J233" s="14"/>
+    </row>
+    <row r="234" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I234" s="14"/>
+      <c r="J234" s="14"/>
+    </row>
+    <row r="235" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I235" s="14"/>
+      <c r="J235" s="14"/>
+    </row>
+    <row r="236" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I236" s="14"/>
+      <c r="J236" s="14"/>
+    </row>
+    <row r="237" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I237" s="14"/>
+      <c r="J237" s="14"/>
+    </row>
+    <row r="238" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I238" s="14"/>
+      <c r="J238" s="14"/>
+    </row>
+    <row r="239" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I239" s="14"/>
+      <c r="J239" s="14"/>
+    </row>
+    <row r="240" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I240" s="14"/>
+      <c r="J240" s="14"/>
+    </row>
+    <row r="241" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I241" s="14"/>
+      <c r="J241" s="14"/>
+    </row>
+    <row r="242" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I242" s="14"/>
+      <c r="J242" s="14"/>
+    </row>
+    <row r="243" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I243" s="14"/>
+      <c r="J243" s="14"/>
+    </row>
+    <row r="244" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I244" s="14"/>
+      <c r="J244" s="14"/>
+    </row>
+    <row r="245" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I245" s="14"/>
+      <c r="J245" s="14"/>
+    </row>
+    <row r="246" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I246" s="14"/>
+      <c r="J246" s="14"/>
+    </row>
+    <row r="247" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I247" s="14"/>
+      <c r="J247" s="14"/>
+    </row>
+    <row r="248" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I248" s="14"/>
+      <c r="J248" s="14"/>
+    </row>
+    <row r="249" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I249" s="14"/>
+      <c r="J249" s="14"/>
+    </row>
+    <row r="250" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I250" s="14"/>
+      <c r="J250" s="14"/>
+    </row>
+    <row r="251" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I251" s="14"/>
+      <c r="J251" s="14"/>
+    </row>
+    <row r="252" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I252" s="14"/>
+      <c r="J252" s="14"/>
+    </row>
+    <row r="253" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I253" s="14"/>
+      <c r="J253" s="14"/>
+    </row>
+    <row r="254" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I254" s="14"/>
+      <c r="J254" s="14"/>
+    </row>
+    <row r="255" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I255" s="14"/>
+      <c r="J255" s="14"/>
+    </row>
+    <row r="256" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I256" s="14"/>
+      <c r="J256" s="14"/>
+    </row>
+    <row r="257" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I257" s="14"/>
+      <c r="J257" s="14"/>
+    </row>
+    <row r="258" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I258" s="14"/>
+      <c r="J258" s="14"/>
+    </row>
+    <row r="259" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I259" s="14"/>
+      <c r="J259" s="14"/>
+    </row>
+    <row r="260" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I260" s="14"/>
+      <c r="J260" s="14"/>
+    </row>
+    <row r="261" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I261" s="14"/>
+      <c r="J261" s="14"/>
+    </row>
+    <row r="262" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I262" s="14"/>
+      <c r="J262" s="14"/>
+    </row>
+    <row r="263" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I263" s="14"/>
+      <c r="J263" s="14"/>
+    </row>
+    <row r="264" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I264" s="14"/>
+      <c r="J264" s="14"/>
+    </row>
+    <row r="265" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I265" s="14"/>
+      <c r="J265" s="14"/>
+    </row>
+    <row r="266" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I266" s="14"/>
+      <c r="J266" s="14"/>
+    </row>
+    <row r="267" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I267" s="14"/>
+      <c r="J267" s="14"/>
+    </row>
+    <row r="268" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I268" s="14"/>
+      <c r="J268" s="14"/>
+    </row>
+    <row r="269" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I269" s="14"/>
+      <c r="J269" s="14"/>
+    </row>
+    <row r="270" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I270" s="14"/>
+      <c r="J270" s="14"/>
+    </row>
+    <row r="271" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I271" s="14"/>
+      <c r="J271" s="14"/>
+    </row>
+    <row r="272" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I272" s="14"/>
+      <c r="J272" s="14"/>
+    </row>
+    <row r="273" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I273" s="14"/>
+      <c r="J273" s="14"/>
+    </row>
+    <row r="274" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I274" s="14"/>
+      <c r="J274" s="14"/>
+    </row>
+    <row r="275" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I275" s="14"/>
+      <c r="J275" s="14"/>
+    </row>
+    <row r="276" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I276" s="14"/>
+      <c r="J276" s="14"/>
+    </row>
+    <row r="277" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I277" s="14"/>
+      <c r="J277" s="14"/>
+    </row>
+    <row r="278" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I278" s="14"/>
+      <c r="J278" s="14"/>
+    </row>
+    <row r="279" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I279" s="14"/>
+      <c r="J279" s="14"/>
+    </row>
+    <row r="280" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I280" s="14"/>
+      <c r="J280" s="14"/>
+    </row>
+    <row r="281" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I281" s="14"/>
+      <c r="J281" s="14"/>
+    </row>
+    <row r="282" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I282" s="14"/>
+      <c r="J282" s="14"/>
+    </row>
+    <row r="283" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I283" s="14"/>
+      <c r="J283" s="14"/>
+    </row>
+    <row r="284" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I284" s="14"/>
+      <c r="J284" s="14"/>
+    </row>
+    <row r="285" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I285" s="14"/>
+      <c r="J285" s="14"/>
+    </row>
+    <row r="286" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I286" s="14"/>
+      <c r="J286" s="14"/>
+    </row>
+    <row r="287" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I287" s="14"/>
+      <c r="J287" s="14"/>
+    </row>
+    <row r="288" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I288" s="14"/>
+      <c r="J288" s="14"/>
+    </row>
+    <row r="289" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I289" s="14"/>
+      <c r="J289" s="14"/>
+    </row>
+    <row r="290" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I290" s="14"/>
+      <c r="J290" s="14"/>
+    </row>
+    <row r="291" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I291" s="14"/>
+      <c r="J291" s="14"/>
+    </row>
+    <row r="292" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I292" s="14"/>
+      <c r="J292" s="14"/>
+    </row>
+    <row r="293" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I293" s="14"/>
+      <c r="J293" s="14"/>
+    </row>
+    <row r="294" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I294" s="14"/>
+      <c r="J294" s="14"/>
+    </row>
+    <row r="295" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I295" s="14"/>
+      <c r="J295" s="14"/>
+    </row>
+    <row r="296" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I296" s="14"/>
+      <c r="J296" s="14"/>
+    </row>
+    <row r="297" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I297" s="14"/>
+      <c r="J297" s="14"/>
+    </row>
+    <row r="298" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I298" s="14"/>
+      <c r="J298" s="14"/>
+    </row>
+    <row r="299" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I299" s="14"/>
+      <c r="J299" s="14"/>
+    </row>
+    <row r="300" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I300" s="14"/>
+      <c r="J300" s="14"/>
+    </row>
+    <row r="301" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I301" s="14"/>
+      <c r="J301" s="14"/>
+    </row>
+    <row r="302" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I302" s="14"/>
+      <c r="J302" s="14"/>
+    </row>
+    <row r="303" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I303" s="14"/>
+      <c r="J303" s="14"/>
+    </row>
+    <row r="304" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I304" s="14"/>
+      <c r="J304" s="14"/>
+    </row>
+    <row r="305" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I305" s="14"/>
+      <c r="J305" s="14"/>
+    </row>
+    <row r="306" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I306" s="14"/>
+      <c r="J306" s="14"/>
+    </row>
+    <row r="307" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I307" s="14"/>
+      <c r="J307" s="14"/>
+    </row>
+    <row r="308" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I308" s="14"/>
+      <c r="J308" s="14"/>
+    </row>
+    <row r="309" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I309" s="14"/>
+      <c r="J309" s="14"/>
+    </row>
+    <row r="310" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I310" s="14"/>
+      <c r="J310" s="14"/>
+    </row>
+    <row r="311" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I311" s="14"/>
+      <c r="J311" s="14"/>
+    </row>
+    <row r="312" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I312" s="14"/>
+      <c r="J312" s="14"/>
+    </row>
+    <row r="313" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I313" s="14"/>
+      <c r="J313" s="14"/>
+    </row>
+    <row r="314" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I314" s="14"/>
+      <c r="J314" s="14"/>
+    </row>
+    <row r="315" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I315" s="14"/>
+      <c r="J315" s="14"/>
+    </row>
+    <row r="316" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I316" s="14"/>
+      <c r="J316" s="14"/>
+    </row>
+    <row r="317" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I317" s="14"/>
+      <c r="J317" s="14"/>
+    </row>
+    <row r="318" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I318" s="14"/>
+      <c r="J318" s="14"/>
+    </row>
+    <row r="319" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I319" s="14"/>
+      <c r="J319" s="14"/>
+    </row>
+    <row r="320" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I320" s="14"/>
+      <c r="J320" s="14"/>
+    </row>
+    <row r="321" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I321" s="14"/>
+      <c r="J321" s="14"/>
+    </row>
+    <row r="322" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I322" s="14"/>
+      <c r="J322" s="14"/>
+    </row>
+    <row r="323" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I323" s="14"/>
+      <c r="J323" s="14"/>
+    </row>
+    <row r="324" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I324" s="14"/>
+      <c r="J324" s="14"/>
+    </row>
+    <row r="325" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I325" s="14"/>
+      <c r="J325" s="14"/>
+    </row>
+    <row r="326" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I326" s="14"/>
+      <c r="J326" s="14"/>
+    </row>
+    <row r="327" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I327" s="14"/>
+      <c r="J327" s="14"/>
+    </row>
+    <row r="328" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I328" s="14"/>
+      <c r="J328" s="14"/>
+    </row>
+    <row r="329" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I329" s="14"/>
+      <c r="J329" s="14"/>
+    </row>
+    <row r="330" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I330" s="14"/>
+      <c r="J330" s="14"/>
+    </row>
+    <row r="331" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I331" s="14"/>
+      <c r="J331" s="14"/>
+    </row>
+    <row r="332" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I332" s="14"/>
+      <c r="J332" s="14"/>
+    </row>
+    <row r="333" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I333" s="14"/>
+      <c r="J333" s="14"/>
+    </row>
+    <row r="334" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I334" s="14"/>
+      <c r="J334" s="14"/>
+    </row>
+    <row r="335" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I335" s="14"/>
+      <c r="J335" s="14"/>
+    </row>
+    <row r="336" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I336" s="14"/>
+      <c r="J336" s="14"/>
+    </row>
+    <row r="337" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I337" s="14"/>
+      <c r="J337" s="14"/>
+    </row>
+    <row r="338" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I338" s="14"/>
+      <c r="J338" s="14"/>
+    </row>
+    <row r="339" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I339" s="14"/>
+      <c r="J339" s="14"/>
+    </row>
+    <row r="340" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I340" s="14"/>
+      <c r="J340" s="14"/>
+    </row>
+    <row r="341" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I341" s="14"/>
+      <c r="J341" s="14"/>
+    </row>
+    <row r="342" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I342" s="14"/>
+      <c r="J342" s="14"/>
+    </row>
+    <row r="343" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I343" s="14"/>
+      <c r="J343" s="14"/>
+    </row>
+    <row r="344" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I344" s="14"/>
+      <c r="J344" s="14"/>
+    </row>
+    <row r="345" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I345" s="14"/>
+      <c r="J345" s="14"/>
+    </row>
+    <row r="346" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I346" s="14"/>
+      <c r="J346" s="14"/>
+    </row>
+    <row r="347" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I347" s="14"/>
+      <c r="J347" s="14"/>
+    </row>
+    <row r="348" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I348" s="14"/>
+      <c r="J348" s="14"/>
+    </row>
+    <row r="349" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I349" s="14"/>
+      <c r="J349" s="14"/>
+    </row>
+    <row r="350" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I350" s="14"/>
+      <c r="J350" s="14"/>
+    </row>
+    <row r="351" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I351" s="14"/>
+      <c r="J351" s="14"/>
+    </row>
+    <row r="352" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I352" s="14"/>
+      <c r="J352" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777778" bottom="1.0527777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E38B838-A91B-46D1-9DB2-76E89AE8A570}">
   <sheetPr>
     <tabColor theme="0" tint="-0.14999847407452621"/>
@@ -2842,19 +4685,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9.109375" style="1"/>
-    <col min="3" max="7" width="9.109375" style="4"/>
-    <col min="8" max="10" width="9.109375" style="1"/>
-    <col min="11" max="11" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="7" width="9.140625" style="4"/>
+    <col min="8" max="10" width="9.140625" style="1"/>
+    <col min="11" max="11" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>55</v>
       </c>
@@ -2903,7 +4746,7 @@
       <c r="AG1" s="9"/>
       <c r="AH1" s="6"/>
     </row>
-    <row r="2" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -2955,7 +4798,7 @@
       <c r="AG2" s="6"/>
       <c r="AH2" s="6"/>
     </row>
-    <row r="3" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F3" s="12"/>
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
@@ -2996,7 +4839,7 @@
       <c r="AX3" s="6"/>
       <c r="AY3" s="6"/>
     </row>
-    <row r="4" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F4" s="12"/>
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
@@ -3037,7 +4880,7 @@
       <c r="AX4" s="6"/>
       <c r="AY4" s="6"/>
     </row>
-    <row r="5" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F5" s="12"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
@@ -3078,7 +4921,7 @@
       <c r="AX5" s="6"/>
       <c r="AY5" s="6"/>
     </row>
-    <row r="6" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -3119,7 +4962,7 @@
       <c r="AX6" s="6"/>
       <c r="AY6" s="6"/>
     </row>
-    <row r="7" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
@@ -3160,7 +5003,7 @@
       <c r="AX7" s="6"/>
       <c r="AY7" s="6"/>
     </row>
-    <row r="8" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F8" s="12"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
@@ -3201,7 +5044,7 @@
       <c r="AX8" s="6"/>
       <c r="AY8" s="6"/>
     </row>
-    <row r="9" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
@@ -3242,7 +5085,7 @@
       <c r="AX9" s="6"/>
       <c r="AY9" s="6"/>
     </row>
-    <row r="10" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F10" s="12"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
@@ -3283,7 +5126,7 @@
       <c r="AX10" s="6"/>
       <c r="AY10" s="6"/>
     </row>
-    <row r="11" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F11" s="12"/>
       <c r="I11" s="12"/>
       <c r="J11" s="12"/>
@@ -3324,7 +5167,7 @@
       <c r="AX11" s="6"/>
       <c r="AY11" s="6"/>
     </row>
-    <row r="12" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F12" s="12"/>
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
@@ -3365,7 +5208,7 @@
       <c r="AX12" s="6"/>
       <c r="AY12" s="6"/>
     </row>
-    <row r="13" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F13" s="12"/>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
@@ -3406,7 +5249,7 @@
       <c r="AX13" s="6"/>
       <c r="AY13" s="6"/>
     </row>
-    <row r="14" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F14" s="12"/>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
@@ -3447,7 +5290,7 @@
       <c r="AX14" s="6"/>
       <c r="AY14" s="6"/>
     </row>
-    <row r="15" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F15" s="12"/>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
@@ -3488,7 +5331,7 @@
       <c r="AX15" s="6"/>
       <c r="AY15" s="6"/>
     </row>
-    <row r="16" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F16" s="12"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
@@ -3529,7 +5372,7 @@
       <c r="AX16" s="6"/>
       <c r="AY16" s="6"/>
     </row>
-    <row r="17" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F17" s="12"/>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
@@ -3570,7 +5413,7 @@
       <c r="AX17" s="6"/>
       <c r="AY17" s="6"/>
     </row>
-    <row r="18" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F18" s="12"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
@@ -3611,90 +5454,90 @@
       <c r="AX18" s="6"/>
       <c r="AY18" s="6"/>
     </row>
-    <row r="19" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F19" s="12"/>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
       <c r="M19" s="13"/>
     </row>
-    <row r="20" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F20" s="12"/>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
       <c r="M20" s="13"/>
     </row>
-    <row r="21" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F21" s="12"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
       <c r="M21" s="13"/>
     </row>
-    <row r="22" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F22" s="12"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
       <c r="M22" s="13"/>
     </row>
-    <row r="23" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F23" s="12"/>
       <c r="I23" s="12"/>
       <c r="J23" s="12"/>
       <c r="M23" s="13"/>
     </row>
-    <row r="24" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F24" s="12"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
       <c r="M24" s="13"/>
     </row>
-    <row r="25" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F25" s="12"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
       <c r="M25" s="13"/>
     </row>
-    <row r="26" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F26" s="12"/>
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
       <c r="M26" s="13"/>
     </row>
-    <row r="27" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F27" s="12"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
       <c r="M27" s="13"/>
     </row>
-    <row r="28" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F28" s="12"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
       <c r="M28" s="13"/>
     </row>
-    <row r="29" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F29" s="12"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
       <c r="M29" s="13"/>
     </row>
-    <row r="30" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="6:51" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="33" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="34" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="35" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="40" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="41" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="42" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="45" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="46" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="47" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3704,7 +5547,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F24F96-793C-4B16-B186-95750A0D0A50}">
   <sheetPr>
     <tabColor theme="0" tint="-0.14999847407452621"/>
@@ -3715,9 +5558,9 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:31" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
@@ -3817,7 +5660,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D74FCD8C-4AE3-4E37-9388-A79339E052B0}">
   <dimension ref="A1:AD1"/>
   <sheetViews>
@@ -3825,9 +5668,9 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:30" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>

</xml_diff>